<commit_message>
Added recent new labs to master, and spreadsheet
Also updated master_supplement, mastersupplement_MT, and the document
outlining changes to the potential labs.
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
@@ -154,6 +154,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="I12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This material is now covered in the "Introduction to Electric Potential" and "Electric Potential for Continuous Charge Distributions"</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I13" authorId="0" shapeId="0">
       <text>
         <r>
@@ -174,11 +198,59 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-I'll admit that this one's pretty weak.  Eventually, something like this content should get folded into a redone version of the main "electric potential" lab.</t>
+I believe this is a more complete introduction to V than the older lab from Dickinson.</t>
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The material in this short lab is now folded into the Introduction to Electric Potential lab.  I consider this example problem lab to be obsolete.  --MT, 2017</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I've personally never been a huge fan of these four labs.  To the extent that they provided a way to visualize V and E, and to think about superposition due to multiple charges, those function are now provided by the two labs "Electric Potential for Multiple Charges: Superposition" and "Electric Potential for Continuous Charge Distributions."</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,32 +297,6 @@
           <t xml:space="preserve">
 cost of books for faculty, for instance.
 (Approximation)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matt Trawick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-My view is that this lab raises conceptual difficulties.  It requires using an AC source, which is hard for students to understand.  The lab tries to get at the relationship between charge and voltage in a capacitor, but it does so mathematically rather than really focusing on building student intuition for what's happening.
-For what it's worth, I recently added some discussion about current to the RC circuit lab, which kind of addresses the question of what's happening to charge as the capacitor voltage increases.  (Though it doesn't directly address the relationship Q = CV.)
-There's also the little detail that one seldom sees capacitors in series outside of contrived intro physics problems, but that's just me.</t>
         </r>
       </text>
     </comment>
@@ -347,11 +393,37 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+My view is that this lab raises conceptual difficulties.  It requires using an AC source, which is hard for students to understand.  The lab tries to get at the relationship between charge and voltage in a capacitor, but it does so mathematically rather than really focusing on building student intuition for what's happening.
+For what it's worth, I recently added some discussion about current to the RC circuit lab, which kind of addresses the question of what's happening to charge as the capacitor voltage increases.  (Though it doesn't directly address the relationship Q = CV.)
+There's also the little detail that one seldom sees capacitors in series outside of contrived intro physics problems, but that's just me.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 This is not the most sophisticated investigation we do, and it takes some time, but OH MY GOD do students LOVE this lab!!! (It also drives home kind of viscerally what this P=IV business really means.)</t>
         </r>
       </text>
     </comment>
-    <comment ref="L27" authorId="0" shapeId="0">
+    <comment ref="L30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O27" authorId="0" shapeId="0">
+    <comment ref="O30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -391,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O28" authorId="0" shapeId="0">
+    <comment ref="O31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -406,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L31" authorId="0" shapeId="0">
+    <comment ref="L34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -430,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L34" authorId="0" shapeId="0">
+    <comment ref="L37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -455,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L37" authorId="0" shapeId="0">
+    <comment ref="L40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L43" authorId="0" shapeId="0">
+    <comment ref="L46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L48" authorId="0" shapeId="0">
+    <comment ref="L51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -527,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L49" authorId="0" shapeId="0">
+    <comment ref="L52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L51" authorId="0" shapeId="0">
+    <comment ref="L54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -576,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N53" authorId="0" shapeId="0">
+    <comment ref="N56" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -600,7 +672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L54" authorId="0" shapeId="0">
+    <comment ref="L57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -625,7 +697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L57" authorId="0" shapeId="0">
+    <comment ref="L60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -649,7 +721,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L60" authorId="0" shapeId="0">
+    <comment ref="L63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -674,7 +746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L69" authorId="0" shapeId="0">
+    <comment ref="L72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -703,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="214">
   <si>
     <t>new, by MT</t>
   </si>
@@ -1078,9 +1150,6 @@
     <t>The Electric Field Near a Charged Rod</t>
   </si>
   <si>
-    <t>The Electric Potential</t>
-  </si>
-  <si>
     <t>An Example Problem Using Electric Potential</t>
   </si>
   <si>
@@ -1337,6 +1406,24 @@
   </si>
   <si>
     <t>by MT, 2017</t>
+  </si>
+  <si>
+    <t>Introduction to Electric Potential</t>
+  </si>
+  <si>
+    <t>The Electric Potential [older lab from Dickinson]</t>
+  </si>
+  <si>
+    <t>Electric Potential for Multiple Charges: Superposition</t>
+  </si>
+  <si>
+    <t>Electric Potential for Continuous Charge Distributions</t>
+  </si>
+  <si>
+    <t>Now Obsolete?</t>
+  </si>
+  <si>
+    <t>by MT, 2015. Now Obsolete?</t>
   </si>
 </sst>
 </file>
@@ -2549,7 +2636,7 @@
   <dimension ref="A1:Y110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2583,16 +2670,16 @@
         <v>87</v>
       </c>
       <c r="E1" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>205</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>206</v>
       </c>
       <c r="I1" s="51" t="s">
         <v>111</v>
@@ -2604,19 +2691,19 @@
         <v>113</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M1" s="49" t="s">
         <v>103</v>
       </c>
       <c r="N1" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="O1" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="O1" s="49" t="s">
-        <v>187</v>
-      </c>
       <c r="P1" s="52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="R1" s="33"/>
@@ -2786,7 +2873,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="14">
         <v>2</v>
@@ -2823,7 +2910,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="77">
-        <f t="shared" ref="P5:P65" si="1">SUM(L5:O5)</f>
+        <f t="shared" ref="P5:P68" si="1">SUM(L5:O5)</f>
         <v>4</v>
       </c>
       <c r="Q5" s="5"/>
@@ -2839,7 +2926,7 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="14">
         <v>2</v>
@@ -2885,7 +2972,7 @@
     <row r="7" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48"/>
       <c r="B7" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7" s="27">
         <v>1</v>
@@ -2898,7 +2985,7 @@
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J7" s="37"/>
       <c r="K7" s="37"/>
@@ -2923,7 +3010,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="14">
         <v>4</v>
@@ -3067,29 +3154,25 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C11" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="E11" s="14">
-        <v>17</v>
-      </c>
       <c r="F11" s="14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11" s="14">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H11" s="14">
-        <v>6</v>
-      </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="2">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
@@ -3124,36 +3207,40 @@
     </row>
     <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>122</v>
+        <v>209</v>
       </c>
       <c r="C12" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D12" s="14">
         <v>0</v>
       </c>
+      <c r="E12" s="14">
+        <v>16</v>
+      </c>
       <c r="F12" s="14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G12" s="14">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H12" s="14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="20">
-        <v>1</v>
+        <v>212</v>
+      </c>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="36">
+        <v>0</v>
       </c>
       <c r="M12" s="34">
         <v>1</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="34">
         <v>1</v>
       </c>
       <c r="O12" s="34">
@@ -3161,7 +3248,7 @@
       </c>
       <c r="P12" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="44">
@@ -3177,38 +3264,28 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="C13" s="14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D13" s="14">
         <v>0</v>
       </c>
-      <c r="F13" s="14">
-        <v>8</v>
-      </c>
-      <c r="H13" s="14">
-        <v>8</v>
-      </c>
       <c r="I13" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L13" s="20">
-        <v>1</v>
-      </c>
-      <c r="M13" s="34">
-        <v>1</v>
-      </c>
-      <c r="O13" s="34">
-        <v>1</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="36">
+        <v>1</v>
+      </c>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="33"/>
@@ -3222,37 +3299,40 @@
     </row>
     <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C14" s="14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>17</v>
+      </c>
+      <c r="F14" s="14">
         <v>6</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>16</v>
-      </c>
-      <c r="F14" s="14">
-        <v>9</v>
-      </c>
       <c r="G14" s="14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" s="14">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I14" s="22"/>
-      <c r="K14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L14" s="20">
+      <c r="J14" s="34">
+        <v>1</v>
+      </c>
+      <c r="K14" s="34">
+        <v>1</v>
+      </c>
+      <c r="L14" s="36">
         <v>1</v>
       </c>
       <c r="M14" s="34">
         <v>1</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="34">
         <v>1</v>
       </c>
       <c r="O14" s="34">
@@ -3275,38 +3355,40 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C15" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D15" s="14">
         <v>0</v>
       </c>
       <c r="F15" s="14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
-      <c r="L15" s="20">
-        <v>1</v>
+        <v>213</v>
+      </c>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="36">
+        <v>0</v>
       </c>
       <c r="M15" s="34">
         <v>1</v>
       </c>
+      <c r="N15" s="34"/>
       <c r="O15" s="34">
         <v>1</v>
       </c>
       <c r="P15" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="17" t="s">
@@ -3324,34 +3406,24 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>126</v>
+        <v>210</v>
       </c>
       <c r="C16" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="14">
-        <v>1</v>
-      </c>
-      <c r="E16" s="14">
-        <v>18</v>
-      </c>
-      <c r="F16" s="14">
-        <v>11</v>
-      </c>
-      <c r="G16" s="14">
-        <v>16</v>
-      </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="2">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="36">
         <v>1</v>
       </c>
       <c r="M16" s="34"/>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
+      <c r="N16" s="34"/>
       <c r="O16" s="34"/>
       <c r="P16" s="77">
         <f t="shared" si="1"/>
@@ -3373,38 +3445,28 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="C17" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="14">
         <v>0</v>
       </c>
-      <c r="E17" s="14">
-        <v>19</v>
-      </c>
-      <c r="F17" s="14">
-        <v>12</v>
-      </c>
-      <c r="G17" s="14">
-        <v>17</v>
-      </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
+      <c r="I17" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="36">
         <v>1</v>
       </c>
       <c r="M17" s="34"/>
-      <c r="N17" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="N17" s="34"/>
       <c r="O17" s="34"/>
       <c r="P17" s="77">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>SUM(L17:O17)</f>
+        <v>1</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="18" t="s">
@@ -3422,38 +3484,38 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D18" s="14">
         <v>0</v>
       </c>
-      <c r="E18" s="14">
-        <v>20</v>
-      </c>
       <c r="F18" s="14">
-        <v>13</v>
-      </c>
-      <c r="G18" s="14">
-        <v>18</v>
-      </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="2">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H18" s="14">
+        <v>10</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
-      <c r="M18" s="34"/>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="O18" s="34"/>
+      <c r="L18" s="20">
+        <v>1</v>
+      </c>
+      <c r="M18" s="34">
+        <v>1</v>
+      </c>
+      <c r="O18" s="34">
+        <v>1</v>
+      </c>
       <c r="P18" s="77">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="18" t="s">
@@ -3471,21 +3533,26 @@
     </row>
     <row r="19" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C19" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="14">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F19" s="14">
-        <v>14</v>
-      </c>
-      <c r="I19" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="G19" s="14">
+        <v>16</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>212</v>
+      </c>
       <c r="J19" s="2">
         <v>1</v>
       </c>
@@ -3493,10 +3560,13 @@
         <v>1</v>
       </c>
       <c r="M19" s="34"/>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
       <c r="O19" s="34"/>
       <c r="P19" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="15"/>
       <c r="R19" s="19" t="s">
@@ -3514,7 +3584,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C20" s="14">
         <v>3</v>
@@ -3523,14 +3593,31 @@
         <v>0</v>
       </c>
       <c r="E20" s="14">
-        <v>22</v>
-      </c>
-      <c r="I20" s="22"/>
+        <v>19</v>
+      </c>
+      <c r="F20" s="14">
+        <v>12</v>
+      </c>
+      <c r="G20" s="14">
+        <v>17</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
       <c r="M20" s="34"/>
-      <c r="O20" s="33"/>
+      <c r="N20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="34"/>
       <c r="P20" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q20" s="15"/>
       <c r="U20" s="33"/>
@@ -3541,28 +3628,40 @@
     </row>
     <row r="21" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="14">
         <v>0</v>
       </c>
       <c r="E21" s="14">
-        <v>23</v>
-      </c>
-      <c r="I21" s="22"/>
-      <c r="L21" s="20">
-        <v>0.4</v>
+        <v>20</v>
+      </c>
+      <c r="F21" s="14">
+        <v>13</v>
+      </c>
+      <c r="G21" s="14">
+        <v>18</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
       </c>
       <c r="M21" s="34"/>
-      <c r="O21" s="34">
-        <v>1</v>
-      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="34"/>
       <c r="P21" s="77">
         <f t="shared" si="1"/>
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
@@ -3576,50 +3675,47 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C22" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="14">
         <v>0</v>
       </c>
       <c r="E22" s="14">
-        <v>24</v>
-      </c>
-      <c r="G22" s="14">
-        <v>23</v>
-      </c>
-      <c r="I22" s="22"/>
+        <v>21</v>
+      </c>
+      <c r="F22" s="14">
+        <v>14</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>212</v>
+      </c>
       <c r="J22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="20">
-        <v>0</v>
+      <c r="K22" s="2">
+        <v>1</v>
       </c>
       <c r="M22" s="34"/>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
-      <c r="O22" s="34">
-        <v>0</v>
-      </c>
+      <c r="O22" s="34"/>
       <c r="P22" s="77">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="S22" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="U22" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="V22" s="33"/>
       <c r="W22" s="33"/>
@@ -3627,66 +3723,40 @@
       <c r="Y22" s="33"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="13">
-        <v>10</v>
-      </c>
-      <c r="D23" s="13">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
-        <v>15</v>
-      </c>
-      <c r="G23" s="13">
-        <v>24</v>
-      </c>
-      <c r="H23" s="13">
-        <v>11</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="L23" s="12">
-        <v>1</v>
-      </c>
-      <c r="M23" s="35">
-        <v>1</v>
-      </c>
-      <c r="N23" s="12">
-        <v>1</v>
-      </c>
-      <c r="O23" s="35">
-        <v>1</v>
-      </c>
-      <c r="P23" s="78">
+      <c r="B23" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="14">
+        <v>3</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14">
+        <v>22</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="M23" s="34"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="15"/>
       <c r="R23" s="81">
         <v>0</v>
       </c>
       <c r="S23" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R23,C$2:C$77)</f>
-        <v>288</v>
+        <f t="shared" ref="S23:S31" si="2">SUMIF(P$2:P$80,"&gt;=" &amp; R23,C$2:C$80)</f>
+        <v>306</v>
       </c>
       <c r="T23" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R23,D$2:D$77)</f>
+        <f t="shared" ref="T23:T31" si="3">SUMIF(P$2:P$80,"&gt;=" &amp; R23,D$2:D$80)</f>
         <v>21</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" ref="U23:U31" si="2">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
-        <v>30.81</v>
+        <f t="shared" ref="U23:U31" si="4">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
+        <v>31.980000000000004</v>
       </c>
       <c r="V23" s="33"/>
       <c r="W23" s="33"/>
@@ -3696,64 +3766,50 @@
     <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C24" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D24" s="14">
         <v>0</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14">
-        <v>16</v>
-      </c>
-      <c r="G24" s="14">
-        <v>25</v>
-      </c>
-      <c r="H24" s="14">
-        <v>12</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
+      <c r="E24" s="14">
+        <v>23</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="20">
-        <v>1</v>
-      </c>
-      <c r="M24" s="34">
-        <v>1</v>
-      </c>
-      <c r="N24" s="2">
-        <v>1</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="M24" s="34"/>
+      <c r="N24" s="2"/>
       <c r="O24" s="34">
         <v>1</v>
       </c>
       <c r="P24" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="81">
         <v>0.5</v>
       </c>
       <c r="S24" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R24,C$2:C$77)</f>
-        <v>196</v>
+        <f t="shared" si="2"/>
+        <v>214</v>
       </c>
       <c r="T24" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R24,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="U24" s="8">
-        <f t="shared" si="2"/>
-        <v>20.150000000000002</v>
+        <f t="shared" si="4"/>
+        <v>21.320000000000004</v>
       </c>
       <c r="V24" s="33"/>
       <c r="W24" s="33"/>
@@ -3762,57 +3818,53 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C25" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="14">
         <v>0</v>
       </c>
-      <c r="F25" s="14">
-        <v>17</v>
-      </c>
-      <c r="H25" s="14">
-        <v>13</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>93</v>
-      </c>
+      <c r="E25" s="14">
+        <v>24</v>
+      </c>
+      <c r="G25" s="14">
+        <v>23</v>
+      </c>
+      <c r="I25" s="22"/>
       <c r="J25" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="K25" s="2">
         <v>1</v>
       </c>
       <c r="L25" s="20">
-        <v>1</v>
-      </c>
-      <c r="M25" s="34">
+        <v>0</v>
+      </c>
+      <c r="M25" s="34"/>
+      <c r="N25" s="2">
         <v>1</v>
       </c>
       <c r="O25" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="15"/>
       <c r="R25" s="81">
         <v>1</v>
       </c>
       <c r="S25" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R25,C$2:C$77)</f>
-        <v>193</v>
+        <f t="shared" si="2"/>
+        <v>211</v>
       </c>
       <c r="T25" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R25,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="U25" s="8">
-        <f t="shared" si="2"/>
-        <v>19.955000000000002</v>
+        <f t="shared" si="4"/>
+        <v>21.125</v>
       </c>
       <c r="V25" s="33"/>
       <c r="W25" s="33"/>
@@ -3820,46 +3872,48 @@
       <c r="Y25" s="33"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B26" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="14">
-        <v>3</v>
-      </c>
-      <c r="D26" s="14">
-        <v>0</v>
-      </c>
-      <c r="F26" s="14">
-        <v>18</v>
-      </c>
-      <c r="G26" s="14">
-        <v>26</v>
-      </c>
-      <c r="H26" s="14">
-        <v>14</v>
-      </c>
-      <c r="I26" s="22" t="s">
+      <c r="A26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="13">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13">
+        <v>15</v>
+      </c>
+      <c r="G26" s="13">
+        <v>24</v>
+      </c>
+      <c r="H26" s="13">
+        <v>11</v>
+      </c>
+      <c r="I26" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="2">
-        <v>1</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1</v>
-      </c>
-      <c r="L26" s="20">
-        <v>1</v>
-      </c>
-      <c r="M26" s="34">
-        <v>1</v>
-      </c>
-      <c r="N26" s="2">
-        <v>1</v>
-      </c>
-      <c r="O26" s="34">
-        <v>1</v>
-      </c>
-      <c r="P26" s="77">
+      <c r="J26" s="12"/>
+      <c r="K26" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="L26" s="12">
+        <v>1</v>
+      </c>
+      <c r="M26" s="35">
+        <v>1</v>
+      </c>
+      <c r="N26" s="12">
+        <v>1</v>
+      </c>
+      <c r="O26" s="35">
+        <v>1</v>
+      </c>
+      <c r="P26" s="78">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3868,15 +3922,15 @@
         <v>1.5</v>
       </c>
       <c r="S26" s="31">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R26,C$2:C$77)</f>
+        <f t="shared" si="2"/>
         <v>163</v>
       </c>
       <c r="T26" s="31">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R26,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U26" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.615000000000002</v>
       </c>
       <c r="V26" s="33"/>
@@ -3886,292 +3940,291 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C27" s="14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D27" s="14">
         <v>0</v>
       </c>
-      <c r="E27" s="14">
-        <v>37</v>
-      </c>
-      <c r="I27" s="22"/>
-      <c r="M27" s="34"/>
+      <c r="F27" s="14">
+        <v>16</v>
+      </c>
+      <c r="G27" s="14">
+        <v>25</v>
+      </c>
+      <c r="H27" s="14">
+        <v>12</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="20">
+        <v>1</v>
+      </c>
+      <c r="M27" s="34">
+        <v>1</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
       <c r="O27" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="81">
         <v>2</v>
       </c>
       <c r="S27" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R27,C$2:C$77)</f>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="T27" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R27,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U27" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.225000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C28" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="14">
         <v>0</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="M28" s="34"/>
+      <c r="F28" s="14">
+        <v>17</v>
+      </c>
+      <c r="H28" s="14">
+        <v>13</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28" s="20">
+        <v>1</v>
+      </c>
+      <c r="M28" s="34">
+        <v>1</v>
+      </c>
       <c r="O28" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="81">
         <v>2.5</v>
       </c>
       <c r="S28" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R28,C$2:C$77)</f>
-        <v>129</v>
+        <f t="shared" si="2"/>
+        <v>128</v>
       </c>
       <c r="T28" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R28,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U28" s="8">
-        <f t="shared" si="2"/>
-        <v>15.404999999999999</v>
+        <f t="shared" si="4"/>
+        <v>15.340000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="13">
+      <c r="B29" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="14">
         <v>3</v>
       </c>
-      <c r="D29" s="13">
-        <v>0</v>
-      </c>
-      <c r="E29" s="13">
-        <v>28</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13">
-        <v>27</v>
-      </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="12">
-        <v>1</v>
-      </c>
-      <c r="O29" s="35"/>
-      <c r="P29" s="78">
+      <c r="D29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
+        <v>18</v>
+      </c>
+      <c r="G29" s="14">
+        <v>26</v>
+      </c>
+      <c r="H29" s="14">
+        <v>14</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="20">
+        <v>1</v>
+      </c>
+      <c r="M29" s="34">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="34">
+        <v>1</v>
+      </c>
+      <c r="P29" s="77">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="81">
         <v>3</v>
       </c>
       <c r="S29" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R29,C$2:C$77)</f>
-        <v>115</v>
+        <f t="shared" si="2"/>
+        <v>114</v>
       </c>
       <c r="T29" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R29,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U29" s="8">
-        <f t="shared" si="2"/>
-        <v>14.495000000000001</v>
+        <f t="shared" si="4"/>
+        <v>14.43</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C30" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D30" s="14">
         <v>0</v>
       </c>
       <c r="E30" s="14">
-        <v>29</v>
-      </c>
-      <c r="F30" s="14">
-        <v>19</v>
-      </c>
-      <c r="G30" s="14">
-        <v>28</v>
-      </c>
-      <c r="H30" s="14">
-        <v>15</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
-      </c>
-      <c r="L30" s="20">
-        <v>1</v>
-      </c>
-      <c r="M30" s="34">
-        <v>1</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="33"/>
+        <v>37</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="M30" s="34"/>
+      <c r="O30" s="34">
+        <v>0</v>
+      </c>
       <c r="P30" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="15"/>
       <c r="R30" s="81">
         <v>3.5</v>
       </c>
       <c r="S30" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R30,C$2:C$77)</f>
-        <v>86</v>
+        <f t="shared" si="2"/>
+        <v>80</v>
       </c>
       <c r="T30" s="6">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R30,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="U30" s="8">
-        <f t="shared" si="2"/>
-        <v>10.66</v>
+        <f t="shared" si="4"/>
+        <v>10.270000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C31" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D31" s="14">
         <v>0</v>
       </c>
-      <c r="E31" s="14">
-        <v>30</v>
-      </c>
-      <c r="F31" s="14">
-        <v>20</v>
-      </c>
-      <c r="G31" s="14">
-        <v>29</v>
-      </c>
-      <c r="H31" s="14">
-        <v>16</v>
-      </c>
-      <c r="I31" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="L31" s="20">
-        <v>1</v>
-      </c>
-      <c r="M31" s="34">
-        <v>1</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
+      <c r="I31" s="22"/>
+      <c r="M31" s="34"/>
       <c r="O31" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="15"/>
       <c r="R31" s="83">
         <v>4</v>
       </c>
       <c r="S31" s="47">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R31,C$2:C$77)</f>
-        <v>71</v>
+        <f t="shared" si="2"/>
+        <v>65</v>
       </c>
       <c r="T31" s="47">
-        <f>SUMIF(P$2:P$77,"&gt;=" &amp; R31,D$2:D$77)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="U31" s="9">
-        <f t="shared" si="2"/>
-        <v>9.6850000000000023</v>
+        <f t="shared" si="4"/>
+        <v>9.2949999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="14">
+      <c r="A32" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="13">
         <v>3</v>
       </c>
-      <c r="D32" s="14">
-        <v>0</v>
-      </c>
-      <c r="E32" s="14">
-        <v>31</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14">
-        <v>30</v>
-      </c>
-      <c r="H32" s="14">
-        <v>17</v>
-      </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="34">
-        <v>1</v>
-      </c>
-      <c r="N32" s="2">
-        <v>1</v>
-      </c>
-      <c r="O32" s="34">
-        <v>0</v>
-      </c>
-      <c r="P32" s="77">
+      <c r="D32" s="13">
+        <v>0</v>
+      </c>
+      <c r="E32" s="13">
+        <v>28</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="12">
+        <v>1</v>
+      </c>
+      <c r="O32" s="35"/>
+      <c r="P32" s="78">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="15"/>
       <c r="R32" s="3"/>
@@ -4180,27 +4233,30 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="C33" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33" s="14">
         <v>0</v>
       </c>
+      <c r="E33" s="14">
+        <v>29</v>
+      </c>
       <c r="F33" s="14">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G33" s="14">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H33" s="14">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="K33" s="2">
+        <v>182</v>
+      </c>
+      <c r="J33" s="2">
         <v>1</v>
       </c>
       <c r="L33" s="20">
@@ -4212,35 +4268,51 @@
       <c r="N33" s="2">
         <v>1</v>
       </c>
-      <c r="O33" s="34">
-        <v>1</v>
-      </c>
+      <c r="O33" s="33"/>
       <c r="P33" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q33" s="15"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C34" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" s="14">
         <v>0</v>
       </c>
+      <c r="E34" s="14">
+        <v>30</v>
+      </c>
+      <c r="F34" s="14">
+        <v>20</v>
+      </c>
+      <c r="G34" s="14">
+        <v>29</v>
+      </c>
       <c r="H34" s="14">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>97</v>
+        <v>183</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1</v>
       </c>
       <c r="L34" s="20">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="M34" s="34">
+        <v>1</v>
+      </c>
+      <c r="N34" s="2">
         <v>1</v>
       </c>
       <c r="O34" s="34">
@@ -4248,13 +4320,13 @@
       </c>
       <c r="P34" s="77">
         <f t="shared" si="1"/>
-        <v>2.7</v>
+        <v>4</v>
       </c>
       <c r="Q34" s="15"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C35" s="14">
         <v>3</v>
@@ -4262,53 +4334,53 @@
       <c r="D35" s="14">
         <v>0</v>
       </c>
+      <c r="E35" s="14">
+        <v>31</v>
+      </c>
+      <c r="G35" s="14">
+        <v>30</v>
+      </c>
       <c r="H35" s="14">
-        <v>20</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="L35" s="20">
-        <v>0.7</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I35" s="22"/>
       <c r="M35" s="34">
         <v>1</v>
       </c>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
       <c r="O35" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" s="77">
         <f t="shared" si="1"/>
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="15"/>
       <c r="R35" s="84"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="C36" s="14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D36" s="14">
         <v>0</v>
       </c>
-      <c r="E36" s="14">
-        <v>33</v>
-      </c>
       <c r="F36" s="14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36" s="14">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H36" s="14">
-        <v>21</v>
-      </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="2">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="K36" s="2">
         <v>1</v>
@@ -4333,54 +4405,33 @@
       <c r="R36" s="84"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C37" s="13">
-        <v>2</v>
-      </c>
-      <c r="D37" s="13">
-        <v>0</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="F37" s="13">
-        <v>23</v>
-      </c>
-      <c r="G37" s="13">
-        <v>33</v>
-      </c>
-      <c r="H37" s="13">
-        <v>22</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="J37" s="12">
-        <v>1</v>
-      </c>
-      <c r="K37" s="12">
+      <c r="B37" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="14">
+        <v>4</v>
+      </c>
+      <c r="D37" s="14">
+        <v>0</v>
+      </c>
+      <c r="H37" s="14">
+        <v>19</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="20">
         <v>0.7</v>
       </c>
-      <c r="L37" s="12">
-        <v>1</v>
-      </c>
-      <c r="M37" s="35">
-        <v>1</v>
-      </c>
-      <c r="N37" s="12">
-        <v>1</v>
-      </c>
-      <c r="O37" s="35">
-        <v>1</v>
-      </c>
-      <c r="P37" s="78">
+      <c r="M37" s="34">
+        <v>1</v>
+      </c>
+      <c r="O37" s="34">
+        <v>1</v>
+      </c>
+      <c r="P37" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="Q37" s="15"/>
       <c r="R37" s="84"/>
@@ -4388,40 +4439,24 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="C38" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D38" s="14">
         <v>0</v>
       </c>
-      <c r="E38" s="14">
-        <v>36</v>
-      </c>
-      <c r="F38" s="14">
-        <v>24</v>
-      </c>
-      <c r="G38" s="14">
-        <v>34</v>
-      </c>
       <c r="H38" s="14">
-        <v>23</v>
-      </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="2">
-        <v>1</v>
-      </c>
-      <c r="K38" s="2">
+        <v>20</v>
+      </c>
+      <c r="I38" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" s="20">
         <v>0.7</v>
       </c>
-      <c r="L38" s="20">
-        <v>1</v>
-      </c>
       <c r="M38" s="34">
-        <v>1</v>
-      </c>
-      <c r="N38" s="2">
         <v>1</v>
       </c>
       <c r="O38" s="34">
@@ -4429,70 +4464,108 @@
       </c>
       <c r="P38" s="77">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="Q38" s="15"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="C39" s="14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D39" s="14">
         <v>0</v>
       </c>
+      <c r="E39" s="14">
+        <v>33</v>
+      </c>
+      <c r="F39" s="14">
+        <v>22</v>
+      </c>
+      <c r="G39" s="14">
+        <v>32</v>
+      </c>
+      <c r="H39" s="14">
+        <v>21</v>
+      </c>
       <c r="I39" s="22"/>
-      <c r="M39" s="34"/>
-      <c r="O39" s="33"/>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39" s="20">
+        <v>1</v>
+      </c>
+      <c r="M39" s="34">
+        <v>1</v>
+      </c>
+      <c r="N39" s="2">
+        <v>1</v>
+      </c>
+      <c r="O39" s="34">
+        <v>1</v>
+      </c>
       <c r="P39" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="6"/>
     </row>
     <row r="40" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="14">
-        <v>6</v>
-      </c>
-      <c r="D40" s="14">
-        <v>0</v>
-      </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14">
-        <v>25</v>
-      </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14">
-        <v>24</v>
-      </c>
-      <c r="I40" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="J40" s="2">
-        <v>1</v>
-      </c>
-      <c r="K40" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L40" s="20">
-        <v>1</v>
-      </c>
-      <c r="M40" s="34"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="34">
-        <v>1</v>
-      </c>
-      <c r="P40" s="77">
+      <c r="A40" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="13">
+        <v>2</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="13">
+        <v>23</v>
+      </c>
+      <c r="G40" s="13">
+        <v>33</v>
+      </c>
+      <c r="H40" s="13">
+        <v>22</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="J40" s="12">
+        <v>1</v>
+      </c>
+      <c r="K40" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="L40" s="12">
+        <v>1</v>
+      </c>
+      <c r="M40" s="35">
+        <v>1</v>
+      </c>
+      <c r="N40" s="12">
+        <v>1</v>
+      </c>
+      <c r="O40" s="35">
+        <v>1</v>
+      </c>
+      <c r="P40" s="78">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="3"/>
@@ -4505,31 +4578,32 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="C41" s="14">
         <v>5</v>
       </c>
       <c r="D41" s="14">
-        <v>2</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>200</v>
+        <v>0</v>
+      </c>
+      <c r="E41" s="14">
+        <v>36</v>
       </c>
       <c r="F41" s="14">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G41" s="14">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H41" s="14">
-        <v>25</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>180</v>
+        <v>23</v>
+      </c>
+      <c r="I41" s="22"/>
+      <c r="J41" s="2">
+        <v>1</v>
       </c>
       <c r="K41" s="2">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="L41" s="20">
         <v>1</v>
@@ -4554,82 +4628,43 @@
       <c r="Y41" s="6"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" s="13">
-        <v>6</v>
-      </c>
-      <c r="D42" s="13">
-        <v>0</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F42" s="13">
-        <v>28</v>
-      </c>
-      <c r="G42" s="13">
-        <v>11</v>
-      </c>
-      <c r="H42" s="13">
-        <v>26</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="J42" s="12">
-        <v>1</v>
-      </c>
-      <c r="K42" s="12">
-        <v>1</v>
-      </c>
-      <c r="L42" s="12">
-        <v>1</v>
-      </c>
-      <c r="M42" s="35">
-        <v>1</v>
-      </c>
-      <c r="N42" s="12">
-        <v>1</v>
-      </c>
-      <c r="O42" s="35">
-        <v>0.8</v>
-      </c>
-      <c r="P42" s="78">
+      <c r="B42" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="14">
+        <v>4</v>
+      </c>
+      <c r="D42" s="14">
+        <v>0</v>
+      </c>
+      <c r="I42" s="22"/>
+      <c r="M42" s="34"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="77">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="U42" s="6"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="C43" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D43" s="14">
         <v>0</v>
       </c>
-      <c r="E43" s="14" t="s">
-        <v>202</v>
-      </c>
       <c r="F43" s="14">
-        <v>29</v>
-      </c>
-      <c r="G43" s="14">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H43" s="14">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="J43" s="2">
         <v>1</v>
@@ -4638,20 +4673,15 @@
         <v>0.5</v>
       </c>
       <c r="L43" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="M43" s="34">
-        <v>1</v>
-      </c>
-      <c r="N43" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M43" s="34"/>
       <c r="O43" s="34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="P43" s="77">
         <f t="shared" si="1"/>
-        <v>3.7</v>
+        <v>2</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
@@ -4659,35 +4689,34 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" s="14">
+        <v>5</v>
+      </c>
+      <c r="D44" s="14">
         <v>2</v>
       </c>
-      <c r="D44" s="14">
-        <v>0</v>
-      </c>
-      <c r="E44" s="14">
-        <v>43</v>
+      <c r="E44" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="F44" s="14">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G44" s="14">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="H44" s="14">
-        <v>28</v>
-      </c>
-      <c r="I44" s="22"/>
-      <c r="J44" s="2">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="I44" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="K44" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L44" s="20">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M44" s="34">
         <v>1</v>
@@ -4696,54 +4725,64 @@
         <v>1</v>
       </c>
       <c r="O44" s="34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="P44" s="77">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="T44" s="6"/>
     </row>
     <row r="45" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="C45" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D45" s="13">
         <v>0</v>
       </c>
-      <c r="E45" s="13">
-        <v>38</v>
+      <c r="E45" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="F45" s="13">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G45" s="13">
-        <v>9</v>
-      </c>
-      <c r="H45" s="13"/>
-      <c r="I45" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="H45" s="13">
+        <v>26</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="J45" s="12">
         <v>1</v>
       </c>
       <c r="K45" s="12">
         <v>1</v>
       </c>
-      <c r="L45" s="12"/>
-      <c r="M45" s="35"/>
+      <c r="L45" s="12">
+        <v>1</v>
+      </c>
+      <c r="M45" s="35">
+        <v>1</v>
+      </c>
       <c r="N45" s="12">
         <v>1</v>
       </c>
-      <c r="O45" s="35"/>
+      <c r="O45" s="35">
+        <v>0.8</v>
+      </c>
       <c r="P45" s="78">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.8</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="3"/>
@@ -4757,124 +4796,139 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B46" s="23" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="C46" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D46" s="14">
         <v>0</v>
       </c>
-      <c r="E46" s="14">
-        <v>39</v>
+      <c r="E46" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="F46" s="14">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G46" s="14">
-        <v>10</v>
-      </c>
-      <c r="I46" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="H46" s="14">
+        <v>27</v>
+      </c>
+      <c r="I46" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="J46" s="2">
         <v>1</v>
       </c>
       <c r="K46" s="2">
-        <v>1</v>
-      </c>
-      <c r="M46" s="34"/>
+        <v>0.5</v>
+      </c>
+      <c r="L46" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M46" s="34">
+        <v>1</v>
+      </c>
       <c r="N46" s="2">
         <v>1</v>
       </c>
-      <c r="O46" s="34"/>
+      <c r="O46" s="34">
+        <v>0.8</v>
+      </c>
       <c r="P46" s="77">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.7</v>
       </c>
       <c r="Q46" s="15"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="C47" s="13">
+      <c r="B47" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="14">
         <v>2</v>
       </c>
-      <c r="D47" s="13">
-        <v>0</v>
-      </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13">
-        <v>33</v>
-      </c>
-      <c r="G47" s="13">
-        <v>1</v>
-      </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="12">
-        <v>1</v>
-      </c>
-      <c r="K47" s="12">
-        <v>1</v>
-      </c>
-      <c r="L47" s="12"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="12">
-        <v>0</v>
-      </c>
-      <c r="O47" s="35">
-        <v>0</v>
-      </c>
-      <c r="P47" s="78">
+      <c r="D47" s="14">
+        <v>0</v>
+      </c>
+      <c r="E47" s="14">
+        <v>43</v>
+      </c>
+      <c r="F47" s="14">
+        <v>30</v>
+      </c>
+      <c r="G47" s="14">
+        <v>13</v>
+      </c>
+      <c r="H47" s="14">
+        <v>28</v>
+      </c>
+      <c r="I47" s="22"/>
+      <c r="J47" s="2">
+        <v>1</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M47" s="34">
+        <v>1</v>
+      </c>
+      <c r="N47" s="2">
+        <v>1</v>
+      </c>
+      <c r="O47" s="34">
+        <v>0.8</v>
+      </c>
+      <c r="P47" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="Q47" s="15"/>
     </row>
     <row r="48" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C48" s="14">
-        <v>4</v>
-      </c>
-      <c r="D48" s="14">
-        <v>0</v>
-      </c>
-      <c r="E48" s="14">
-        <v>2</v>
-      </c>
-      <c r="F48" s="14">
-        <v>34</v>
-      </c>
-      <c r="G48" s="14">
-        <v>6</v>
-      </c>
-      <c r="H48" s="14">
-        <v>30</v>
-      </c>
-      <c r="I48" s="22"/>
-      <c r="J48" s="2">
-        <v>1</v>
-      </c>
-      <c r="K48" s="2">
-        <v>1</v>
-      </c>
-      <c r="L48" s="20"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="2">
-        <v>1</v>
-      </c>
-      <c r="O48" s="85">
-        <v>1</v>
-      </c>
-      <c r="P48" s="77">
+      <c r="A48" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="13">
+        <v>3</v>
+      </c>
+      <c r="D48" s="13">
+        <v>0</v>
+      </c>
+      <c r="E48" s="13">
+        <v>38</v>
+      </c>
+      <c r="F48" s="13">
+        <v>31</v>
+      </c>
+      <c r="G48" s="13">
+        <v>9</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="12">
+        <v>1</v>
+      </c>
+      <c r="K48" s="12">
+        <v>1</v>
+      </c>
+      <c r="L48" s="12"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="12">
+        <v>1</v>
+      </c>
+      <c r="O48" s="35"/>
+      <c r="P48" s="78">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
@@ -4886,37 +4940,38 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C49" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" s="14">
         <v>0</v>
       </c>
       <c r="E49" s="14">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="F49" s="14">
+        <v>32</v>
       </c>
       <c r="G49" s="14">
-        <v>2</v>
-      </c>
-      <c r="H49" s="14">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="I49" s="22"/>
       <c r="J49" s="2">
         <v>1</v>
       </c>
+      <c r="K49" s="2">
+        <v>1</v>
+      </c>
       <c r="M49" s="34"/>
       <c r="N49" s="2">
         <v>1</v>
       </c>
-      <c r="O49" s="85">
-        <v>1</v>
-      </c>
+      <c r="O49" s="34"/>
       <c r="P49" s="77">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="15"/>
       <c r="V49" s="33"/>
@@ -4925,36 +4980,44 @@
       <c r="Y49" s="6"/>
     </row>
     <row r="50" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C50" s="14">
-        <v>3</v>
-      </c>
-      <c r="D50" s="14">
-        <v>0</v>
-      </c>
-      <c r="E50" s="14">
-        <v>5</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="2">
-        <v>1</v>
-      </c>
-      <c r="K50" s="2"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="85">
-        <v>1</v>
-      </c>
-      <c r="P50" s="77">
+      <c r="A50" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="13">
+        <v>2</v>
+      </c>
+      <c r="D50" s="13">
+        <v>0</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13">
+        <v>33</v>
+      </c>
+      <c r="G50" s="13">
+        <v>1</v>
+      </c>
+      <c r="H50" s="13"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="12">
+        <v>1</v>
+      </c>
+      <c r="K50" s="12">
+        <v>1</v>
+      </c>
+      <c r="L50" s="12"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="12">
+        <v>0</v>
+      </c>
+      <c r="O50" s="35">
+        <v>0</v>
+      </c>
+      <c r="P50" s="78">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="15"/>
       <c r="R50" s="3"/>
@@ -4968,33 +5031,34 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C51" s="14">
+        <v>4</v>
+      </c>
+      <c r="D51" s="14">
+        <v>0</v>
+      </c>
+      <c r="E51" s="14">
         <v>2</v>
       </c>
-      <c r="D51" s="14">
-        <v>0</v>
-      </c>
-      <c r="E51" s="14">
+      <c r="F51" s="14">
+        <v>34</v>
+      </c>
+      <c r="G51" s="14">
         <v>6</v>
       </c>
-      <c r="G51" s="14">
-        <v>3</v>
-      </c>
       <c r="H51" s="14">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I51" s="22"/>
       <c r="J51" s="2">
         <v>1</v>
       </c>
-      <c r="L51" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="M51" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="M51" s="34"/>
       <c r="N51" s="2">
         <v>1</v>
       </c>
@@ -5003,90 +5067,72 @@
       </c>
       <c r="P51" s="77">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="V51" s="33"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C52" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" s="14">
-        <v>8</v>
-      </c>
-      <c r="F52" s="14">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G52" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H52" s="14">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I52" s="22"/>
-      <c r="K52" s="2">
-        <v>1</v>
-      </c>
-      <c r="L52" s="20">
-        <v>1</v>
-      </c>
-      <c r="M52" s="34">
-        <v>1</v>
-      </c>
+      <c r="J52" s="2">
+        <v>1</v>
+      </c>
+      <c r="M52" s="34"/>
       <c r="N52" s="2">
         <v>1</v>
       </c>
-      <c r="O52" s="33"/>
+      <c r="O52" s="85">
+        <v>1</v>
+      </c>
       <c r="P52" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q52" s="15"/>
       <c r="V52" s="33"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C53" s="14">
+        <v>3</v>
+      </c>
+      <c r="D53" s="14">
+        <v>0</v>
+      </c>
+      <c r="E53" s="14">
         <v>5</v>
       </c>
-      <c r="D53" s="14">
-        <v>0</v>
-      </c>
-      <c r="E53" s="14">
-        <v>9</v>
-      </c>
-      <c r="F53" s="14">
-        <v>36</v>
-      </c>
-      <c r="G53" s="14">
-        <v>5</v>
-      </c>
-      <c r="H53" s="14">
-        <v>34</v>
-      </c>
       <c r="I53" s="22"/>
-      <c r="L53" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="M53" s="34">
-        <v>1</v>
-      </c>
-      <c r="N53" s="2">
-        <v>1</v>
-      </c>
-      <c r="O53" s="33"/>
+      <c r="J53" s="2">
+        <v>1</v>
+      </c>
+      <c r="M53" s="34"/>
+      <c r="O53" s="85">
+        <v>1</v>
+      </c>
       <c r="P53" s="77">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="T53" s="6"/>
@@ -5094,33 +5140,34 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C54" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="14">
         <v>0</v>
       </c>
-      <c r="F54" s="14">
-        <v>37</v>
+      <c r="E54" s="14">
+        <v>6</v>
+      </c>
+      <c r="G54" s="14">
+        <v>3</v>
       </c>
       <c r="H54" s="14">
-        <v>35</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>115</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I54" s="22"/>
       <c r="J54" s="2">
         <v>1</v>
       </c>
-      <c r="K54" s="2">
-        <v>1</v>
-      </c>
       <c r="L54" s="20">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="M54" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="N54" s="2">
         <v>1</v>
       </c>
       <c r="O54" s="85">
@@ -5128,37 +5175,50 @@
       </c>
       <c r="P54" s="77">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="Q54" s="15"/>
       <c r="V54" s="33"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="C55" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D55" s="14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E55" s="14">
+        <v>8</v>
+      </c>
+      <c r="F55" s="14">
+        <v>35</v>
+      </c>
+      <c r="G55" s="14">
+        <v>4</v>
       </c>
       <c r="H55" s="14">
-        <v>36</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>97</v>
+        <v>33</v>
+      </c>
+      <c r="I55" s="22"/>
+      <c r="K55" s="2">
+        <v>1</v>
       </c>
       <c r="L55" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M55" s="34">
+        <v>1</v>
+      </c>
+      <c r="N55" s="2">
         <v>1</v>
       </c>
       <c r="O55" s="33"/>
       <c r="P55" s="77">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="U55" s="6"/>
@@ -5166,7 +5226,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C56" s="14">
         <v>5</v>
@@ -5174,50 +5234,73 @@
       <c r="D56" s="14">
         <v>0</v>
       </c>
+      <c r="E56" s="14">
+        <v>9</v>
+      </c>
+      <c r="F56" s="14">
+        <v>36</v>
+      </c>
+      <c r="G56" s="14">
+        <v>5</v>
+      </c>
       <c r="H56" s="14">
-        <v>37</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>93</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I56" s="22"/>
       <c r="L56" s="20">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="M56" s="34">
         <v>1</v>
       </c>
-      <c r="O56" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="N56" s="2">
+        <v>1</v>
+      </c>
+      <c r="O56" s="33"/>
       <c r="P56" s="77">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q56" s="15"/>
       <c r="V56" s="33"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C57" s="14">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D57" s="14">
-        <v>2</v>
-      </c>
-      <c r="E57" s="14">
-        <v>10</v>
-      </c>
-      <c r="I57" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="14">
+        <v>37</v>
+      </c>
+      <c r="H57" s="14">
+        <v>35</v>
+      </c>
+      <c r="I57" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J57" s="2">
+        <v>1</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1</v>
+      </c>
       <c r="L57" s="20">
-        <v>0</v>
-      </c>
-      <c r="M57" s="34"/>
-      <c r="O57" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="M57" s="34">
+        <v>1</v>
+      </c>
+      <c r="O57" s="85">
+        <v>1</v>
+      </c>
       <c r="P57" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q57" s="15"/>
       <c r="V57" s="33"/>
@@ -5227,30 +5310,37 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
       <c r="C58" s="14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D58" s="14">
-        <v>1</v>
-      </c>
-      <c r="E58" s="14">
-        <v>11</v>
-      </c>
-      <c r="I58" s="22"/>
-      <c r="M58" s="34"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="14">
+        <v>36</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="L58" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="M58" s="34">
+        <v>1</v>
+      </c>
       <c r="O58" s="33"/>
       <c r="P58" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q58" s="15"/>
       <c r="V58" s="33"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C59" s="14">
         <v>5</v>
@@ -5259,10 +5349,10 @@
         <v>0</v>
       </c>
       <c r="H59" s="14">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L59" s="20">
         <v>1</v>
@@ -5270,74 +5360,55 @@
       <c r="M59" s="34">
         <v>1</v>
       </c>
-      <c r="O59" s="34"/>
+      <c r="O59" s="34">
+        <v>0.5</v>
+      </c>
       <c r="P59" s="77">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Q59" s="15"/>
       <c r="U59" s="6"/>
       <c r="V59" s="33"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="C60" s="13">
-        <v>3</v>
-      </c>
-      <c r="D60" s="13">
-        <v>0</v>
-      </c>
-      <c r="E60" s="13">
-        <v>45</v>
-      </c>
-      <c r="F60" s="13">
-        <v>27</v>
-      </c>
-      <c r="G60" s="13">
-        <v>36</v>
-      </c>
-      <c r="H60" s="13">
-        <v>29</v>
-      </c>
-      <c r="I60" s="21"/>
-      <c r="J60" s="12">
-        <v>1</v>
-      </c>
-      <c r="K60" s="12">
-        <v>1</v>
-      </c>
-      <c r="L60" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="M60" s="35"/>
-      <c r="N60" s="12">
-        <v>1</v>
-      </c>
-      <c r="O60" s="35"/>
-      <c r="P60" s="78">
+      <c r="B60" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" s="14">
+        <v>9</v>
+      </c>
+      <c r="D60" s="14">
+        <v>2</v>
+      </c>
+      <c r="E60" s="14">
+        <v>10</v>
+      </c>
+      <c r="I60" s="22"/>
+      <c r="L60" s="20">
+        <v>0</v>
+      </c>
+      <c r="M60" s="34"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="77">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="15"/>
       <c r="V60" s="33"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C61" s="14">
         <v>7</v>
       </c>
       <c r="D61" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" s="14">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="I61" s="22"/>
       <c r="M61" s="34"/>
@@ -5350,55 +5421,76 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C62" s="14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D62" s="14">
-        <v>2</v>
-      </c>
-      <c r="E62" s="14">
-        <v>47</v>
-      </c>
-      <c r="I62" s="22"/>
-      <c r="M62" s="34"/>
-      <c r="O62" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="14">
+        <v>38</v>
+      </c>
+      <c r="I62" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L62" s="20">
+        <v>1</v>
+      </c>
+      <c r="M62" s="34">
+        <v>1</v>
+      </c>
+      <c r="O62" s="34"/>
       <c r="P62" s="77">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q62" s="15"/>
     </row>
     <row r="63" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="10"/>
-      <c r="B63" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C63" s="14">
-        <v>10</v>
-      </c>
-      <c r="D63" s="14">
-        <v>0</v>
-      </c>
-      <c r="E63" s="14">
-        <v>34</v>
-      </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2">
-        <v>1</v>
-      </c>
-      <c r="L63" s="20"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="34"/>
-      <c r="P63" s="77">
+      <c r="A63" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C63" s="13">
+        <v>3</v>
+      </c>
+      <c r="D63" s="13">
+        <v>0</v>
+      </c>
+      <c r="E63" s="13">
+        <v>45</v>
+      </c>
+      <c r="F63" s="13">
+        <v>27</v>
+      </c>
+      <c r="G63" s="13">
+        <v>36</v>
+      </c>
+      <c r="H63" s="13">
+        <v>29</v>
+      </c>
+      <c r="I63" s="21"/>
+      <c r="J63" s="12">
+        <v>1</v>
+      </c>
+      <c r="K63" s="12">
+        <v>1</v>
+      </c>
+      <c r="L63" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="M63" s="35"/>
+      <c r="N63" s="12">
+        <v>1</v>
+      </c>
+      <c r="O63" s="35"/>
+      <c r="P63" s="78">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q63" s="15"/>
       <c r="R63" s="3"/>
@@ -5411,32 +5503,22 @@
       <c r="Y63"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B64" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="13">
-        <v>6</v>
-      </c>
-      <c r="D64" s="13">
+      <c r="B64" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" s="14">
+        <v>7</v>
+      </c>
+      <c r="D64" s="14">
         <v>2</v>
       </c>
-      <c r="E64" s="13">
-        <v>32</v>
-      </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="78">
+      <c r="E64" s="14">
+        <v>46</v>
+      </c>
+      <c r="I64" s="22"/>
+      <c r="M64" s="34"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5446,16 +5528,16 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B65" s="23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C65" s="14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D65" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E65" s="14">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I65" s="22"/>
       <c r="M65" s="34"/>
@@ -5472,52 +5554,57 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C66" s="14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D66" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="14">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="I66" s="22"/>
+      <c r="K66" s="2">
+        <v>1</v>
+      </c>
       <c r="M66" s="34"/>
-      <c r="O66" s="33"/>
+      <c r="O66" s="34"/>
       <c r="P66" s="77">
-        <f t="shared" ref="P66:P76" si="3">SUM(L66:O66)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q66" s="15"/>
     </row>
     <row r="67" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="10"/>
-      <c r="B67" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C67" s="14">
-        <v>4</v>
-      </c>
-      <c r="D67" s="14">
-        <v>0</v>
-      </c>
-      <c r="E67" s="14">
-        <v>48</v>
-      </c>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="34"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="33"/>
-      <c r="P67" s="77">
-        <f t="shared" si="3"/>
+      <c r="A67" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="13">
+        <v>6</v>
+      </c>
+      <c r="D67" s="13">
+        <v>2</v>
+      </c>
+      <c r="E67" s="13">
+        <v>32</v>
+      </c>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="35"/>
+      <c r="P67" s="78">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q67" s="15"/>
@@ -5532,7 +5619,7 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B68" s="23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C68" s="14">
         <v>3</v>
@@ -5541,77 +5628,58 @@
         <v>0</v>
       </c>
       <c r="E68" s="14">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I68" s="22"/>
       <c r="M68" s="34"/>
-      <c r="O68" s="34"/>
+      <c r="O68" s="33"/>
       <c r="P68" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q68" s="15"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B69" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="13">
-        <v>2</v>
-      </c>
-      <c r="D69" s="13">
-        <v>0</v>
-      </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="12">
-        <v>1</v>
-      </c>
-      <c r="K69" s="12">
-        <v>1</v>
-      </c>
-      <c r="L69" s="12">
-        <v>1</v>
-      </c>
-      <c r="M69" s="35">
-        <v>1</v>
-      </c>
-      <c r="N69" s="12">
-        <v>1</v>
-      </c>
-      <c r="O69" s="35"/>
-      <c r="P69" s="78">
-        <f t="shared" si="3"/>
-        <v>3</v>
+      <c r="B69" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C69" s="14">
+        <v>4</v>
+      </c>
+      <c r="D69" s="14">
+        <v>1</v>
+      </c>
+      <c r="E69" s="14">
+        <v>7</v>
+      </c>
+      <c r="I69" s="22"/>
+      <c r="M69" s="34"/>
+      <c r="O69" s="33"/>
+      <c r="P69" s="77">
+        <f t="shared" ref="P69:P79" si="5">SUM(L69:O69)</f>
+        <v>0</v>
       </c>
       <c r="Q69" s="15"/>
       <c r="T69" s="33"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A70" s="30"/>
-      <c r="B70" s="31" t="s">
-        <v>102</v>
+      <c r="B70" s="23" t="s">
+        <v>168</v>
       </c>
       <c r="C70" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D70" s="14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E70" s="14">
+        <v>48</v>
       </c>
       <c r="I70" s="22"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="M70" s="36"/>
-      <c r="N70" s="20"/>
-      <c r="O70" s="36"/>
+      <c r="M70" s="34"/>
+      <c r="O70" s="33"/>
       <c r="P70" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q70" s="15"/>
@@ -5622,71 +5690,62 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B71" s="23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C71" s="14">
+        <v>3</v>
+      </c>
+      <c r="D71" s="14">
+        <v>0</v>
+      </c>
+      <c r="E71" s="14">
+        <v>49</v>
+      </c>
+      <c r="I71" s="22"/>
+      <c r="M71" s="34"/>
+      <c r="O71" s="34"/>
+      <c r="P71" s="77">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="15"/>
+    </row>
+    <row r="72" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="13">
         <v>2</v>
       </c>
-      <c r="D71" s="14">
-        <v>1</v>
-      </c>
-      <c r="I71" s="22"/>
-      <c r="J71" s="2">
-        <v>1</v>
-      </c>
-      <c r="K71" s="2">
-        <v>1</v>
-      </c>
-      <c r="L71" s="20">
-        <v>1</v>
-      </c>
-      <c r="M71" s="34">
-        <v>1</v>
-      </c>
-      <c r="N71" s="2">
-        <v>1</v>
-      </c>
-      <c r="O71" s="33"/>
-      <c r="P71" s="77">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="Q71" s="15"/>
-    </row>
-    <row r="72" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
-      <c r="B72" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="C72" s="14">
-        <v>4</v>
-      </c>
-      <c r="D72" s="14">
-        <v>3</v>
-      </c>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="2">
-        <v>1</v>
-      </c>
-      <c r="K72" s="2">
-        <v>1</v>
-      </c>
-      <c r="L72" s="20">
-        <v>1</v>
-      </c>
-      <c r="M72" s="34">
-        <v>1</v>
-      </c>
-      <c r="N72" s="2">
-        <v>1</v>
-      </c>
-      <c r="O72" s="33"/>
-      <c r="P72" s="77">
-        <f t="shared" si="3"/>
+      <c r="D72" s="13">
+        <v>0</v>
+      </c>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="12">
+        <v>1</v>
+      </c>
+      <c r="K72" s="12">
+        <v>1</v>
+      </c>
+      <c r="L72" s="12">
+        <v>1</v>
+      </c>
+      <c r="M72" s="35">
+        <v>1</v>
+      </c>
+      <c r="N72" s="12">
+        <v>1</v>
+      </c>
+      <c r="O72" s="35"/>
+      <c r="P72" s="78">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="Q72" s="15"/>
@@ -5700,34 +5759,25 @@
       <c r="Y72"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B73" s="23" t="s">
-        <v>174</v>
+      <c r="A73" s="30"/>
+      <c r="B73" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="C73" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" s="14">
-        <v>0</v>
-      </c>
-      <c r="I73" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="K73" s="2">
-        <v>1</v>
-      </c>
-      <c r="L73" s="20">
-        <v>1</v>
-      </c>
-      <c r="M73" s="34">
-        <v>1</v>
-      </c>
-      <c r="N73" s="2">
-        <v>1</v>
-      </c>
-      <c r="O73" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="I73" s="22"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="M73" s="36"/>
+      <c r="N73" s="20"/>
+      <c r="O73" s="36"/>
       <c r="P73" s="77">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="V73" s="6"/>
@@ -5737,39 +5787,67 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B74" s="23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C74" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="14">
         <v>1</v>
       </c>
       <c r="I74" s="22"/>
-      <c r="M74" s="34"/>
+      <c r="J74" s="2">
+        <v>1</v>
+      </c>
+      <c r="K74" s="2">
+        <v>1</v>
+      </c>
+      <c r="L74" s="20">
+        <v>1</v>
+      </c>
+      <c r="M74" s="34">
+        <v>1</v>
+      </c>
+      <c r="N74" s="2">
+        <v>1</v>
+      </c>
       <c r="O74" s="33"/>
       <c r="P74" s="77">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="Q74" s="15"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B75" s="23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C75" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D75" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I75" s="22"/>
-      <c r="M75" s="34"/>
+      <c r="J75" s="2">
+        <v>1</v>
+      </c>
+      <c r="K75" s="2">
+        <v>1</v>
+      </c>
+      <c r="L75" s="20">
+        <v>1</v>
+      </c>
+      <c r="M75" s="34">
+        <v>1</v>
+      </c>
+      <c r="N75" s="2">
+        <v>1</v>
+      </c>
       <c r="O75" s="33"/>
       <c r="P75" s="77">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="V75" s="6"/>
@@ -5778,234 +5856,260 @@
       <c r="Y75" s="6"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B76" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C76" s="27">
+      <c r="B76" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" s="14">
+        <v>1</v>
+      </c>
+      <c r="D76" s="14">
+        <v>0</v>
+      </c>
+      <c r="I76" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="K76" s="2">
+        <v>1</v>
+      </c>
+      <c r="L76" s="20">
+        <v>1</v>
+      </c>
+      <c r="M76" s="34">
+        <v>1</v>
+      </c>
+      <c r="N76" s="2">
+        <v>1</v>
+      </c>
+      <c r="O76" s="33"/>
+      <c r="P76" s="77">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="Q76" s="15"/>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B77" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" s="14">
+        <v>3</v>
+      </c>
+      <c r="D77" s="14">
+        <v>1</v>
+      </c>
+      <c r="I77" s="22"/>
+      <c r="M77" s="34"/>
+      <c r="O77" s="33"/>
+      <c r="P77" s="77">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q77" s="15"/>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B78" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="14">
+        <v>1</v>
+      </c>
+      <c r="D78" s="14">
+        <v>0</v>
+      </c>
+      <c r="I78" s="22"/>
+      <c r="M78" s="34"/>
+      <c r="O78" s="33"/>
+      <c r="P78" s="77">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q78" s="15"/>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B79" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" s="27">
         <v>4</v>
       </c>
-      <c r="D76" s="27">
-        <v>0</v>
-      </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="29"/>
-      <c r="J76" s="28"/>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="37"/>
-      <c r="N76" s="28"/>
-      <c r="O76" s="37"/>
-      <c r="P76" s="79">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q76" s="15"/>
-    </row>
-    <row r="77" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="11"/>
-      <c r="Q77" s="15"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I78" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="J78" s="65">
-        <f t="array" ref="J78">SUM($C2:$C76*(J2:J76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>87</v>
-      </c>
-      <c r="K78" s="65">
-        <f t="array" ref="K78">SUM($C2:$C76*(K2:K76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>72</v>
-      </c>
-      <c r="L78" s="65">
-        <f t="array" ref="L78">SUM($C2:$C76*(L2:L76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>127</v>
-      </c>
-      <c r="M78" s="65">
-        <f t="array" ref="M78">SUM($C2:$C76*(M2:M76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>145</v>
-      </c>
-      <c r="N78" s="65">
-        <f t="array" ref="N78">SUM($C2:$C76*(N2:N76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>125</v>
-      </c>
-      <c r="O78" s="66">
-        <f t="array" ref="O78">SUM($C2:$C76*(O2:O76&gt;=0.9)*($P2:$P76&gt;=$R$12))</f>
-        <v>107</v>
-      </c>
-      <c r="Q78" s="15"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I79" s="67" t="s">
-        <v>190</v>
-      </c>
-      <c r="J79" s="68">
-        <f t="array" ref="J79">SUM($C2:$C76*J2:J76*($P2:$P76&gt;=$R$12))</f>
-        <v>88.5</v>
-      </c>
-      <c r="K79" s="68">
-        <f t="array" ref="K79">SUM($C2:$C76*K2:K76*($P2:$P76&gt;=$R$12))</f>
-        <v>95.4</v>
-      </c>
-      <c r="L79" s="68">
-        <f t="array" ref="L79">SUM($C2:$C76*L2:L76*($P2:$P76&gt;=$R$12))</f>
-        <v>138.79999999999998</v>
-      </c>
-      <c r="M79" s="68">
-        <f t="array" ref="M79">SUM($C2:$C76*M2:M76*($P2:$P76&gt;=$R$12))</f>
-        <v>146</v>
-      </c>
-      <c r="N79" s="68">
-        <f t="array" ref="N79">SUM($C2:$C76*N2:N76*($P2:$P76&gt;=$R$12))</f>
-        <v>125</v>
-      </c>
-      <c r="O79" s="69">
-        <f t="array" ref="O79">SUM($C2:$C76*O2:O76*($P2:$P76&gt;=$R$12))</f>
-        <v>119.89999999999999</v>
+      <c r="D79" s="27">
+        <v>0</v>
+      </c>
+      <c r="E79" s="27"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="28"/>
+      <c r="O79" s="37"/>
+      <c r="P79" s="79">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="Q79" s="15"/>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I80" s="67" t="s">
-        <v>189</v>
-      </c>
-      <c r="J80" s="68">
-        <f t="array" ref="J80">SUM($C$2:$C$76*(J$2:J$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>90</v>
-      </c>
-      <c r="K80" s="68">
-        <f t="array" ref="K80">SUM($C$2:$C$76*(K$2:K$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>112</v>
-      </c>
-      <c r="L80" s="68">
-        <f t="array" ref="L80">SUM($C$2:$C$76*(L$2:L$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>153</v>
-      </c>
-      <c r="M80" s="68">
-        <f t="array" ref="M80">SUM($C$2:$C$76*(M$2:M$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>147</v>
-      </c>
-      <c r="N80" s="68">
-        <f t="array" ref="N80">SUM($C$2:$C$76*(N$2:N$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>125</v>
-      </c>
-      <c r="O80" s="69">
-        <f t="array" ref="O80">SUM($C$2:$C$76*(O$2:O$76&gt;=0.1)*($P$2:$P$76&gt;=$R$12))</f>
-        <v>125</v>
-      </c>
+    <row r="80" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="11"/>
       <c r="Q80" s="15"/>
       <c r="U80" s="33"/>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I81" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="J81" s="68">
-        <f t="shared" ref="J81:O81" si="4">LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>163</v>
-      </c>
-      <c r="K81" s="68">
-        <f t="shared" si="4"/>
-        <v>163</v>
-      </c>
-      <c r="L81" s="68">
-        <f t="shared" si="4"/>
-        <v>163</v>
-      </c>
-      <c r="M81" s="68">
-        <f t="shared" si="4"/>
-        <v>163</v>
-      </c>
-      <c r="N81" s="68">
-        <f t="shared" si="4"/>
-        <v>163</v>
-      </c>
-      <c r="O81" s="69">
-        <f t="shared" si="4"/>
-        <v>163</v>
+      <c r="I81" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="J81" s="65">
+        <f t="array" ref="J81">SUM($C2:$C79*(J2:J79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>87</v>
+      </c>
+      <c r="K81" s="65">
+        <f t="array" ref="K81">SUM($C2:$C79*(K2:K79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>72</v>
+      </c>
+      <c r="L81" s="65">
+        <f t="array" ref="L81">SUM($C2:$C79*(L2:L79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>120</v>
+      </c>
+      <c r="M81" s="65">
+        <f t="array" ref="M81">SUM($C2:$C79*(M2:M79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>145</v>
+      </c>
+      <c r="N81" s="65">
+        <f t="array" ref="N81">SUM($C2:$C79*(N2:N79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>125</v>
+      </c>
+      <c r="O81" s="66">
+        <f t="array" ref="O81">SUM($C2:$C79*(O2:O79&gt;=0.9)*($P2:$P79&gt;=$R$12))</f>
+        <v>107</v>
       </c>
       <c r="Q81" s="15"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I82" s="67" t="s">
-        <v>192</v>
-      </c>
-      <c r="J82" s="70">
-        <f t="shared" ref="J82:O82" si="5">J79/J81</f>
-        <v>0.54294478527607359</v>
-      </c>
-      <c r="K82" s="70">
-        <f t="shared" si="5"/>
-        <v>0.58527607361963196</v>
-      </c>
-      <c r="L82" s="70">
-        <f t="shared" si="5"/>
-        <v>0.8515337423312882</v>
-      </c>
-      <c r="M82" s="70">
-        <f t="shared" si="5"/>
-        <v>0.89570552147239269</v>
-      </c>
-      <c r="N82" s="70">
-        <f t="shared" si="5"/>
-        <v>0.76687116564417179</v>
-      </c>
-      <c r="O82" s="71">
-        <f t="shared" si="5"/>
-        <v>0.73558282208588954</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C83" s="33"/>
-      <c r="I83" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="J83" s="73">
-        <f t="array" ref="J83">SUM($C2:$C76*J2:J76*($P2:$P76&lt;$R$12))</f>
-        <v>30</v>
-      </c>
-      <c r="K83" s="73">
-        <f t="array" ref="K83">SUM($C2:$C76*K2:K76*($P2:$P76&lt;$R$12))</f>
-        <v>35</v>
-      </c>
-      <c r="L83" s="73">
-        <f t="array" ref="L83">SUM($C2:$C76*L2:L76*($P2:$P76&lt;$R$12))</f>
-        <v>2.6</v>
-      </c>
-      <c r="M83" s="73">
-        <f t="array" ref="M83">SUM($C2:$C76*M2:M76*($P2:$P76&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="N83" s="73">
-        <f t="array" ref="N83">SUM($C2:$C76*N2:N76*($P2:$P76&lt;$R$12))</f>
-        <v>23.5</v>
-      </c>
-      <c r="O83" s="74">
-        <f t="array" ref="O83">SUM($C2:$C76*O2:O76*($P2:$P76&lt;$R$12))</f>
-        <v>7</v>
+        <v>189</v>
+      </c>
+      <c r="J82" s="68">
+        <f t="array" ref="J82">SUM($C2:$C79*J2:J79*($P2:$P79&gt;=$R$12))</f>
+        <v>88.5</v>
+      </c>
+      <c r="K82" s="68">
+        <f t="array" ref="K82">SUM($C2:$C79*K2:K79*($P2:$P79&gt;=$R$12))</f>
+        <v>95.4</v>
+      </c>
+      <c r="L82" s="68">
+        <f t="array" ref="L82">SUM($C2:$C79*L2:L79*($P2:$P79&gt;=$R$12))</f>
+        <v>131.79999999999998</v>
+      </c>
+      <c r="M82" s="68">
+        <f t="array" ref="M82">SUM($C2:$C79*M2:M79*($P2:$P79&gt;=$R$12))</f>
+        <v>146</v>
+      </c>
+      <c r="N82" s="68">
+        <f t="array" ref="N82">SUM($C2:$C79*N2:N79*($P2:$P79&gt;=$R$12))</f>
+        <v>125</v>
+      </c>
+      <c r="O82" s="69">
+        <f t="array" ref="O82">SUM($C2:$C79*O2:O79*($P2:$P79&gt;=$R$12))</f>
+        <v>119.89999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I83" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="J83" s="68">
+        <f t="array" ref="J83">SUM($C$2:$C$79*(J$2:J$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>90</v>
+      </c>
+      <c r="K83" s="68">
+        <f t="array" ref="K83">SUM($C$2:$C$79*(K$2:K$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>112</v>
+      </c>
+      <c r="L83" s="68">
+        <f t="array" ref="L83">SUM($C$2:$C$79*(L$2:L$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>146</v>
+      </c>
+      <c r="M83" s="68">
+        <f t="array" ref="M83">SUM($C$2:$C$79*(M$2:M$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>147</v>
+      </c>
+      <c r="N83" s="68">
+        <f t="array" ref="N83">SUM($C$2:$C$79*(N$2:N$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>125</v>
+      </c>
+      <c r="O83" s="69">
+        <f t="array" ref="O83">SUM($C$2:$C$79*(O$2:O$79&gt;=0.1)*($P$2:$P$79&gt;=$R$12))</f>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C84" s="33"/>
+      <c r="I84" s="67" t="s">
+        <v>190</v>
+      </c>
+      <c r="J84" s="68">
+        <f t="shared" ref="J84:O84" si="6">LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+        <v>163</v>
+      </c>
+      <c r="K84" s="68">
+        <f t="shared" si="6"/>
+        <v>163</v>
+      </c>
+      <c r="L84" s="68">
+        <f t="shared" si="6"/>
+        <v>163</v>
+      </c>
+      <c r="M84" s="68">
+        <f t="shared" si="6"/>
+        <v>163</v>
+      </c>
+      <c r="N84" s="68">
+        <f t="shared" si="6"/>
+        <v>163</v>
+      </c>
+      <c r="O84" s="69">
+        <f t="shared" si="6"/>
+        <v>163</v>
+      </c>
     </row>
     <row r="85" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="23"/>
+      <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
-      <c r="I85" s="20"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="20"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="2"/>
+      <c r="I85" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="J85" s="70">
+        <f t="shared" ref="J85:O85" si="7">J82/J84</f>
+        <v>0.54294478527607359</v>
+      </c>
+      <c r="K85" s="70">
+        <f t="shared" si="7"/>
+        <v>0.58527607361963196</v>
+      </c>
+      <c r="L85" s="70">
+        <f t="shared" si="7"/>
+        <v>0.80858895705521461</v>
+      </c>
+      <c r="M85" s="70">
+        <f t="shared" si="7"/>
+        <v>0.89570552147239269</v>
+      </c>
+      <c r="N85" s="70">
+        <f t="shared" si="7"/>
+        <v>0.76687116564417179</v>
+      </c>
+      <c r="O85" s="71">
+        <f t="shared" si="7"/>
+        <v>0.73558282208588954</v>
+      </c>
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
@@ -6017,14 +6121,48 @@
       <c r="X85"/>
       <c r="Y85"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="33"/>
+      <c r="I86" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="J86" s="73">
+        <f t="array" ref="J86">SUM($C2:$C79*J2:J79*($P2:$P79&lt;$R$12))</f>
+        <v>30</v>
+      </c>
+      <c r="K86" s="73">
+        <f t="array" ref="K86">SUM($C2:$C79*K2:K79*($P2:$P79&lt;$R$12))</f>
+        <v>35</v>
+      </c>
+      <c r="L86" s="73">
+        <f t="array" ref="L86">SUM($C2:$C79*L2:L79*($P2:$P79&lt;$R$12))</f>
+        <v>20.6</v>
+      </c>
+      <c r="M86" s="73">
+        <f t="array" ref="M86">SUM($C2:$C79*M2:M79*($P2:$P79&lt;$R$12))</f>
+        <v>0</v>
+      </c>
+      <c r="N86" s="73">
+        <f t="array" ref="N86">SUM($C2:$C79*N2:N79*($P2:$P79&lt;$R$12))</f>
+        <v>23.5</v>
+      </c>
+      <c r="O86" s="74">
+        <f t="array" ref="O86">SUM($C2:$C79*O2:O79*($P2:$P79&lt;$R$12))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C87" s="33"/>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C88" s="33"/>
       <c r="V88" s="6"/>
       <c r="W88" s="6"/>
       <c r="X88" s="6"/>
       <c r="Y88" s="6"/>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C89" s="33"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="V92" s="6"/>
@@ -6045,7 +6183,7 @@
       <c r="Y110" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P76">
+  <conditionalFormatting sqref="B2:P79">
     <cfRule type="expression" dxfId="2" priority="28" stopIfTrue="1">
       <formula>$P2&gt;=(0.5+$R$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Renamed carbon paper lab
To make it clear that it's a measurement, since it's surrounded by
theory labs.
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
@@ -1450,7 +1450,7 @@
     <t>by MT, 2015. Now Obsolete?</t>
   </si>
   <si>
-    <t>Electric Fields and Equipotential Lines [carbon paper]</t>
+    <t>Measuring Equipotential Lines and Electric Fields [carbon paper]</t>
   </si>
 </sst>
 </file>
@@ -2662,14 +2662,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="14" customWidth="1"/>
     <col min="4" max="8" width="5.88671875" style="14" customWidth="1"/>
     <col min="9" max="9" width="28.44140625" style="20" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
master and spreadsheet updated for fall 2017
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2017fall.xlsx
@@ -15,7 +15,7 @@
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -25,7 +25,7 @@
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,13 +123,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-I wonder if this lab isn't a better fit for 131 than 132.  (The last activity is about circular motion.)  
+I believe this lab is a better fit for 131 than 132.  (The last activity is about circular motion.)  
 I think that this lab takes a lot of time and that the two main learning objectives (the form of the force law and the size of the coulomb constant) can be more efficiently dealt with in lecture or a homework problem.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="S11" authorId="0" shapeId="0">
+    <comment ref="T11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -302,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T19" authorId="0" shapeId="0">
+    <comment ref="U19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,30 +324,6 @@
           <t xml:space="preserve">
 cost of books for faculty, for instance.
 (Approximation)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matt Trawick:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is kind of a "what if" table.  What if we set the cutoff at 2 people using a particular lab for whether to include that lab in the manual?  For each possible cutoff, this table shows how long the manual would be and how much it would cost.</t>
         </r>
       </text>
     </comment>
@@ -371,11 +347,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Resulting number of pages in the manual.</t>
+This is kind of a "what if" table.  What if we set the cutoff at 2 people using a particular lab for whether to include that lab in the manual?  For each possible cutoff, this table shows how long the manual would be and how much it would cost.</t>
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0" shapeId="0">
+    <comment ref="T22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Resulting number of pages in the manual.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -450,6 +450,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="I30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt Trawick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LR and LRC labs still written to use Datastudio.  Also, we haven't run these labs since sometime before 2004, and I'm not even sure we still have the equipment that's listed.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L30" authorId="0" shapeId="0">
       <text>
         <r>
@@ -549,7 +573,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This lab is now ONLY the oscilloscope-and-bar-magnet lab.
+This lab is now ONLY the oscilloscope-and-bar-magnet experiment.
 </t>
         </r>
       </text>
@@ -842,7 +866,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-I love this lab, and I've used it in the past when I've taught Modern Physics.  (It's a nice way to tie those pesky "energy quanta" to something more tangible.)  I tend not to use this in 132, just because I'd rather focus time on other topics. </t>
+I love this lab, and I've used it in the past when I've taught Modern Physics.  (It's a nice way to tie those pesky "energy quanta" to something more tangible.)  I tend not to use this in 132, just because I don't usually have time to do any topics in quantum mechanics.</t>
         </r>
       </text>
     </comment>
@@ -871,7 +895,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L73" authorId="0" shapeId="0">
+    <comment ref="L70" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -900,7 +924,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="214">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1380,15 +1404,6 @@
     <t>Nuclear Decay and Radiocarbon Dating</t>
   </si>
   <si>
-    <t>Centripetal Force</t>
-  </si>
-  <si>
-    <t>Conservation of Angular Momentum</t>
-  </si>
-  <si>
-    <t>Impulse, Momentum, and Interactions</t>
-  </si>
-  <si>
     <t>Galilean Relativity</t>
   </si>
   <si>
@@ -1396,9 +1411,6 @@
   </si>
   <si>
     <t>Treatment of Experimental Data</t>
-  </si>
-  <si>
-    <t>Introduction to DataStudio</t>
   </si>
   <si>
     <t>Introduction to Excel</t>
@@ -1552,6 +1564,15 @@
   </si>
   <si>
     <t>apparatus for 7(?) setups max</t>
+  </si>
+  <si>
+    <t>Not updated for Capstone</t>
+  </si>
+  <si>
+    <t>Not updated for Tracker</t>
+  </si>
+  <si>
+    <t>2017 fall Shaun</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2204,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2383,6 +2404,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2761,10 +2800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y111"/>
+  <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,14 +2816,15 @@
     <col min="10" max="11" width="8.77734375" style="2" customWidth="1"/>
     <col min="12" max="12" width="8.77734375" style="20" customWidth="1"/>
     <col min="13" max="15" width="8.77734375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11" style="3" customWidth="1"/>
-    <col min="17" max="17" width="2.44140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="9.5546875" customWidth="1"/>
-    <col min="21" max="21" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="34" customWidth="1"/>
+    <col min="17" max="17" width="11" style="3" customWidth="1"/>
+    <col min="18" max="18" width="2.44140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.5546875" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>76</v>
       </c>
@@ -2798,16 +2838,16 @@
         <v>86</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I1" s="51" t="s">
         <v>108</v>
@@ -2819,31 +2859,34 @@
         <v>110</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M1" s="49" t="s">
         <v>100</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O1" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="32"/>
+        <v>174</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="R1" s="32"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="32"/>
       <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
+      <c r="V1" s="32"/>
       <c r="W1" s="33"/>
       <c r="X1" s="33"/>
       <c r="Y1" s="33"/>
-    </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z1" s="33"/>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>104</v>
       </c>
@@ -2879,21 +2922,24 @@
       <c r="O2" s="55">
         <v>1</v>
       </c>
-      <c r="P2" s="75">
-        <f t="shared" ref="P2:P3" si="0">SUM(L2:O2)</f>
-        <v>4</v>
-      </c>
-      <c r="Q2" s="80"/>
+      <c r="P2" s="91">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="75">
+        <f>SUM(P2)</f>
+        <v>1</v>
+      </c>
       <c r="R2" s="80"/>
       <c r="S2" s="80"/>
       <c r="T2" s="80"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="33"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="32"/>
       <c r="W2" s="33"/>
       <c r="X2" s="33"/>
       <c r="Y2" s="33"/>
-    </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z2" s="33"/>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48"/>
       <c r="B3" s="54" t="s">
         <v>106</v>
@@ -2927,21 +2973,24 @@
       <c r="O3" s="60">
         <v>1</v>
       </c>
-      <c r="P3" s="76">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q3" s="80"/>
+      <c r="P3" s="92">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="76">
+        <f t="shared" ref="Q3:Q66" si="0">SUM(P3)</f>
+        <v>1</v>
+      </c>
       <c r="R3" s="80"/>
       <c r="S3" s="80"/>
       <c r="T3" s="80"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="33"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="32"/>
       <c r="W3" s="33"/>
       <c r="X3" s="33"/>
       <c r="Y3" s="33"/>
-    </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z3" s="33"/>
+    </row>
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>73</v>
       </c>
@@ -2985,23 +3034,26 @@
       <c r="O4" s="36">
         <v>1</v>
       </c>
-      <c r="P4" s="77">
-        <f>SUM(L4:O4)</f>
-        <v>4</v>
-      </c>
-      <c r="Q4" s="5"/>
+      <c r="P4" s="89">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="33"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="15"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z4" s="33"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C5" s="14">
         <v>2</v>
@@ -3037,24 +3089,27 @@
       <c r="O5" s="85">
         <v>1</v>
       </c>
-      <c r="P5" s="77">
-        <f t="shared" ref="P5:P69" si="1">SUM(L5:O5)</f>
-        <v>4</v>
-      </c>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="33"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="15"/>
       <c r="W5" s="33"/>
       <c r="X5" s="33"/>
       <c r="Y5" s="33"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z5" s="33"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C6" s="14">
         <v>2</v>
@@ -3083,24 +3138,27 @@
         <v>0</v>
       </c>
       <c r="O6" s="6"/>
-      <c r="P6" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="89">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="33"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="15"/>
       <c r="W6" s="33"/>
       <c r="X6" s="33"/>
       <c r="Y6" s="33"/>
-    </row>
-    <row r="7" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z6" s="33"/>
+    </row>
+    <row r="7" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48"/>
       <c r="B7" s="24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C7" s="27">
         <v>1</v>
@@ -3113,7 +3171,7 @@
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="29" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J7" s="37"/>
       <c r="K7" s="37"/>
@@ -3123,22 +3181,25 @@
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
       <c r="O7" s="86"/>
-      <c r="P7" s="79">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="15"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="U7" s="5"/>
+      <c r="V7" s="15"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C8" s="14">
         <v>4</v>
@@ -3153,7 +3214,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
@@ -3169,21 +3230,24 @@
       <c r="O8" s="34">
         <v>1</v>
       </c>
-      <c r="P8" s="77">
-        <f t="shared" si="1"/>
-        <v>3.5</v>
-      </c>
-      <c r="Q8" s="5"/>
+      <c r="P8" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="77">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="33"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="15"/>
       <c r="W8" s="33"/>
       <c r="X8" s="33"/>
       <c r="Y8" s="33"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8" s="33"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>114</v>
       </c>
@@ -3218,21 +3282,24 @@
       <c r="O9" s="34">
         <v>1</v>
       </c>
-      <c r="P9" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q9" s="5"/>
+      <c r="P9" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="33"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="15"/>
       <c r="W9" s="33"/>
       <c r="X9" s="33"/>
       <c r="Y9" s="33"/>
-    </row>
-    <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z9" s="33"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>115</v>
       </c>
@@ -3266,21 +3333,24 @@
         <v>1</v>
       </c>
       <c r="O10" s="33"/>
-      <c r="P10" s="77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="5"/>
+      <c r="P10" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="77">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="33"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="15"/>
       <c r="W10" s="33"/>
       <c r="X10" s="33"/>
       <c r="Y10" s="33"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z10" s="33"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>116</v>
       </c>
@@ -3317,25 +3387,28 @@
       <c r="O11" s="34">
         <v>1</v>
       </c>
-      <c r="P11" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="42" t="s">
+      <c r="P11" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R11" s="5"/>
+      <c r="S11" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="S11" s="43"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="33"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="15"/>
       <c r="W11" s="33"/>
       <c r="X11" s="33"/>
       <c r="Y11" s="33"/>
-    </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z11" s="33"/>
+    </row>
+    <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C12" s="14">
         <v>6</v>
@@ -3356,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J12" s="34"/>
       <c r="K12" s="34">
@@ -3374,25 +3447,28 @@
       <c r="O12" s="34">
         <v>0</v>
       </c>
-      <c r="P12" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="44">
-        <v>1.5</v>
-      </c>
-      <c r="S12" s="45"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="33"/>
+      <c r="P12" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="15"/>
+      <c r="S12" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="T12" s="45"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="15"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
       <c r="Y12" s="33"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z12" s="33"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C13" s="14">
         <v>9</v>
@@ -3401,7 +3477,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
@@ -3413,23 +3489,26 @@
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
-      <c r="P13" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="33"/>
+      <c r="P13" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R13" s="5"/>
       <c r="S13" s="33"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="15"/>
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
       <c r="Y13" s="33"/>
-    </row>
-    <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z13" s="33"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C14" s="14">
         <v>3</v>
@@ -3468,22 +3547,25 @@
       <c r="O14" s="34">
         <v>1</v>
       </c>
-      <c r="P14" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="1" t="s">
+      <c r="P14" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="5"/>
+      <c r="S14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="T14" s="33"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="15"/>
       <c r="W14" s="33"/>
       <c r="X14" s="33"/>
       <c r="Y14" s="33"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z14" s="33"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>117</v>
       </c>
@@ -3500,7 +3582,7 @@
         <v>8</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="34">
@@ -3516,27 +3598,30 @@
       <c r="O15" s="34">
         <v>0</v>
       </c>
-      <c r="P15" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="17" t="s">
+      <c r="P15" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="5"/>
+      <c r="S15" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="S15" s="38"/>
-      <c r="T15" s="16">
+      <c r="T15" s="38"/>
+      <c r="U15" s="16">
         <v>0.05</v>
       </c>
-      <c r="U15" s="33"/>
       <c r="V15" s="33"/>
       <c r="W15" s="33"/>
       <c r="X15" s="33"/>
       <c r="Y15" s="33"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z15" s="33"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C16" s="14">
         <v>5</v>
@@ -3545,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -3557,27 +3642,30 @@
       </c>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
-      <c r="P16" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="18" t="s">
+      <c r="P16" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="5"/>
+      <c r="S16" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="S16" s="5"/>
-      <c r="T16" s="8">
+      <c r="T16" s="5"/>
+      <c r="U16" s="8">
         <v>0.3</v>
       </c>
-      <c r="U16" s="33"/>
       <c r="V16" s="33"/>
       <c r="W16" s="33"/>
       <c r="X16" s="33"/>
       <c r="Y16" s="33"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z16" s="33"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C17" s="14">
         <v>4</v>
@@ -3586,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -3600,25 +3688,28 @@
       <c r="O17" s="34">
         <v>1</v>
       </c>
-      <c r="P17" s="77">
-        <f>SUM(L17:O17)</f>
+      <c r="P17" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="T17" s="5"/>
+      <c r="U17" s="8">
         <v>3</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="S17" s="5"/>
-      <c r="T17" s="8">
-        <v>3</v>
-      </c>
-      <c r="U17" s="33"/>
       <c r="V17" s="33"/>
       <c r="W17" s="33"/>
       <c r="X17" s="33"/>
       <c r="Y17" s="33"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17" s="33"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>118</v>
       </c>
@@ -3649,25 +3740,28 @@
       <c r="O18" s="34">
         <v>1</v>
       </c>
-      <c r="P18" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="18" t="s">
+      <c r="P18" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R18" s="5"/>
+      <c r="S18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="S18" s="5"/>
-      <c r="T18" s="39">
+      <c r="T18" s="5"/>
+      <c r="U18" s="39">
         <v>0.25</v>
       </c>
-      <c r="U18" s="33"/>
       <c r="V18" s="33"/>
       <c r="W18" s="33"/>
       <c r="X18" s="33"/>
       <c r="Y18" s="33"/>
-    </row>
-    <row r="19" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z18" s="33"/>
+    </row>
+    <row r="19" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>119</v>
       </c>
@@ -3687,7 +3781,7 @@
         <v>16</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -3700,25 +3794,28 @@
         <v>1</v>
       </c>
       <c r="O19" s="34"/>
-      <c r="P19" s="77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="19" t="s">
+      <c r="P19" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="15"/>
+      <c r="S19" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="S19" s="40"/>
-      <c r="T19" s="41">
+      <c r="T19" s="40"/>
+      <c r="U19" s="41">
         <v>0.05</v>
       </c>
-      <c r="U19" s="33"/>
       <c r="V19" s="33"/>
       <c r="W19" s="33"/>
       <c r="X19" s="33"/>
       <c r="Y19" s="33"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z19" s="33"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>120</v>
       </c>
@@ -3738,7 +3835,7 @@
         <v>17</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -3751,18 +3848,21 @@
         <v>0.5</v>
       </c>
       <c r="O20" s="34"/>
-      <c r="P20" s="77">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q20" s="15"/>
-      <c r="U20" s="33"/>
+      <c r="P20" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="15"/>
       <c r="V20" s="33"/>
       <c r="W20" s="33"/>
       <c r="X20" s="33"/>
       <c r="Y20" s="33"/>
-    </row>
-    <row r="21" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z20" s="33"/>
+    </row>
+    <row r="21" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
         <v>121</v>
       </c>
@@ -3782,7 +3882,7 @@
         <v>18</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
@@ -3795,21 +3895,24 @@
         <v>1</v>
       </c>
       <c r="O21" s="34"/>
-      <c r="P21" s="77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q21" s="15"/>
+      <c r="P21" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R21" s="15"/>
-      <c r="S21" s="6"/>
+      <c r="S21" s="15"/>
       <c r="T21" s="6"/>
-      <c r="U21" s="33"/>
+      <c r="U21" s="6"/>
       <c r="V21" s="33"/>
       <c r="W21" s="33"/>
       <c r="X21" s="33"/>
       <c r="Y21" s="33"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21" s="33"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>122</v>
       </c>
@@ -3826,7 +3929,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -3836,29 +3939,32 @@
       </c>
       <c r="M22" s="34"/>
       <c r="O22" s="34"/>
-      <c r="P22" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>186</v>
+      <c r="P22" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="46" t="s">
+        <v>181</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="V22" s="33"/>
+        <v>182</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>184</v>
+      </c>
       <c r="W22" s="33"/>
       <c r="X22" s="33"/>
       <c r="Y22" s="33"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22" s="33"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>123</v>
       </c>
@@ -3874,32 +3980,35 @@
       <c r="I23" s="22"/>
       <c r="M23" s="34"/>
       <c r="O23" s="33"/>
-      <c r="P23" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="81">
-        <v>0</v>
-      </c>
-      <c r="S23" s="6">
-        <f t="shared" ref="S23:S31" si="2">SUMIF(P$2:P$81,"&gt;=" &amp; R23,C$2:C$81)</f>
-        <v>305</v>
+      <c r="P23" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="15"/>
+      <c r="S23" s="81">
+        <v>0</v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" ref="T23:T31" si="3">SUMIF(P$2:P$81,"&gt;=" &amp; R23,D$2:D$81)</f>
-        <v>21</v>
-      </c>
-      <c r="U23" s="8">
-        <f t="shared" ref="U23:U31" si="4">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
-        <v>31.915000000000003</v>
-      </c>
-      <c r="V23" s="33"/>
+        <f t="shared" ref="T23:T31" si="1">SUMIF(Q$2:Q$77,"&gt;=" &amp; S23,C$2:C$77)</f>
+        <v>290</v>
+      </c>
+      <c r="U23" s="6">
+        <f t="shared" ref="U23:U31" si="2">SUMIF(Q$2:Q$77,"&gt;=" &amp; S23,D$2:D$77)</f>
+        <v>17</v>
+      </c>
+      <c r="V23" s="8">
+        <f t="shared" ref="V23:V31" si="3">($U$17 + $U$15*T23+$U$16*U23)*(1+U$18+U$19)</f>
+        <v>29.380000000000003</v>
+      </c>
       <c r="W23" s="33"/>
       <c r="X23" s="33"/>
       <c r="Y23" s="33"/>
-    </row>
-    <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="33"/>
+    </row>
+    <row r="24" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
         <v>124</v>
@@ -3927,32 +4036,35 @@
       <c r="O24" s="34">
         <v>1</v>
       </c>
-      <c r="P24" s="77">
+      <c r="P24" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="15"/>
+      <c r="S24" s="81">
+        <v>0.5</v>
+      </c>
+      <c r="T24" s="6">
         <f t="shared" si="1"/>
-        <v>1.4</v>
-      </c>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="S24" s="6">
+        <v>154</v>
+      </c>
+      <c r="U24" s="6">
         <f t="shared" si="2"/>
-        <v>206</v>
-      </c>
-      <c r="T24" s="6">
+        <v>7</v>
+      </c>
+      <c r="V24" s="8">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="U24" s="8">
-        <f t="shared" si="4"/>
-        <v>20.8</v>
-      </c>
-      <c r="V24" s="33"/>
+        <v>16.64</v>
+      </c>
       <c r="W24" s="33"/>
       <c r="X24" s="33"/>
       <c r="Y24" s="33"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z24" s="33"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>125</v>
       </c>
@@ -3982,32 +4094,35 @@
       <c r="O25" s="34">
         <v>0</v>
       </c>
-      <c r="P25" s="77">
+      <c r="P25" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R25" s="15"/>
+      <c r="S25" s="81">
+        <v>1</v>
+      </c>
+      <c r="T25" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="81">
-        <v>1</v>
-      </c>
-      <c r="S25" s="6">
+        <v>119</v>
+      </c>
+      <c r="U25" s="6">
         <f t="shared" si="2"/>
-        <v>203</v>
-      </c>
-      <c r="T25" s="6">
+        <v>7</v>
+      </c>
+      <c r="V25" s="8">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="U25" s="8">
-        <f t="shared" si="4"/>
-        <v>20.605</v>
-      </c>
-      <c r="V25" s="33"/>
+        <v>14.364999999999998</v>
+      </c>
       <c r="W25" s="33"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="33"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z25" s="33"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>75</v>
       </c>
@@ -4049,32 +4164,35 @@
       <c r="O26" s="35">
         <v>1</v>
       </c>
-      <c r="P26" s="78">
+      <c r="P26" s="88">
+        <v>0.7</v>
+      </c>
+      <c r="Q26" s="78">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="R26" s="15"/>
+      <c r="S26" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="T26" s="31">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="S26" s="31">
+        <v>0</v>
+      </c>
+      <c r="U26" s="31">
         <f t="shared" si="2"/>
-        <v>173</v>
-      </c>
-      <c r="T26" s="31">
+        <v>0</v>
+      </c>
+      <c r="V26" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="U26" s="8">
-        <f t="shared" si="4"/>
-        <v>18.265000000000001</v>
-      </c>
-      <c r="V26" s="33"/>
+        <v>3.9000000000000004</v>
+      </c>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
       <c r="Y26" s="33"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z26" s="33"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>127</v>
       </c>
@@ -4114,28 +4232,31 @@
       <c r="O27" s="34">
         <v>1</v>
       </c>
-      <c r="P27" s="77">
+      <c r="P27" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R27" s="15"/>
+      <c r="S27" s="81">
+        <v>2</v>
+      </c>
+      <c r="T27" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="81">
-        <v>2</v>
-      </c>
-      <c r="S27" s="6">
+        <v>0</v>
+      </c>
+      <c r="U27" s="6">
         <f t="shared" si="2"/>
-        <v>167</v>
-      </c>
-      <c r="T27" s="6">
+        <v>0</v>
+      </c>
+      <c r="V27" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="U27" s="8">
-        <f t="shared" si="4"/>
-        <v>17.875</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>128</v>
       </c>
@@ -4169,28 +4290,31 @@
       <c r="O28" s="34">
         <v>1</v>
       </c>
-      <c r="P28" s="77">
+      <c r="P28" s="87">
+        <v>0.7</v>
+      </c>
+      <c r="Q28" s="77">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="R28" s="15"/>
+      <c r="S28" s="81">
+        <v>2.5</v>
+      </c>
+      <c r="T28" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="81">
-        <v>2.5</v>
-      </c>
-      <c r="S28" s="6">
+        <v>0</v>
+      </c>
+      <c r="U28" s="6">
         <f t="shared" si="2"/>
-        <v>129</v>
-      </c>
-      <c r="T28" s="6">
+        <v>0</v>
+      </c>
+      <c r="V28" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="U28" s="8">
-        <f t="shared" si="4"/>
-        <v>15.404999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
         <v>129</v>
       </c>
@@ -4230,28 +4354,31 @@
       <c r="O29" s="34">
         <v>1</v>
       </c>
-      <c r="P29" s="77">
+      <c r="P29" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R29" s="15"/>
+      <c r="S29" s="81">
+        <v>3</v>
+      </c>
+      <c r="T29" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="81">
-        <v>3</v>
-      </c>
-      <c r="S29" s="6">
+        <v>0</v>
+      </c>
+      <c r="U29" s="6">
         <f t="shared" si="2"/>
-        <v>119</v>
-      </c>
-      <c r="T29" s="6">
+        <v>0</v>
+      </c>
+      <c r="V29" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="U29" s="8">
-        <f t="shared" si="4"/>
-        <v>14.755000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>130</v>
       </c>
@@ -4264,33 +4391,38 @@
       <c r="E30" s="14">
         <v>37</v>
       </c>
-      <c r="I30" s="22"/>
+      <c r="I30" s="57" t="s">
+        <v>211</v>
+      </c>
       <c r="M30" s="34"/>
       <c r="O30" s="34">
         <v>0</v>
       </c>
-      <c r="P30" s="77">
+      <c r="P30" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="15"/>
+      <c r="S30" s="81">
+        <v>3.5</v>
+      </c>
+      <c r="T30" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="81">
-        <v>3.5</v>
-      </c>
-      <c r="S30" s="6">
+      <c r="U30" s="6">
         <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="T30" s="6">
+        <v>0</v>
+      </c>
+      <c r="V30" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="U30" s="8">
-        <f t="shared" si="4"/>
-        <v>10.270000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
         <v>131</v>
       </c>
@@ -4300,33 +4432,38 @@
       <c r="D31" s="14">
         <v>0</v>
       </c>
-      <c r="I31" s="22"/>
+      <c r="I31" s="57" t="s">
+        <v>211</v>
+      </c>
       <c r="M31" s="34"/>
       <c r="O31" s="34">
         <v>0</v>
       </c>
-      <c r="P31" s="77">
+      <c r="P31" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="15"/>
+      <c r="S31" s="83">
+        <v>4</v>
+      </c>
+      <c r="T31" s="47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="83">
-        <v>4</v>
-      </c>
-      <c r="S31" s="47">
+      <c r="U31" s="47">
         <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="T31" s="47">
+        <v>0</v>
+      </c>
+      <c r="V31" s="9">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="U31" s="9">
-        <f t="shared" si="4"/>
-        <v>9.2949999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>77</v>
       </c>
@@ -4348,7 +4485,7 @@
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="21" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -4358,16 +4495,19 @@
         <v>1</v>
       </c>
       <c r="O32" s="35"/>
-      <c r="P32" s="78">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="3"/>
-      <c r="S32"/>
+      <c r="P32" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R32" s="15"/>
+      <c r="S32" s="3"/>
       <c r="T32"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="U32"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
         <v>133</v>
       </c>
@@ -4390,7 +4530,7 @@
         <v>15</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J33" s="2">
         <v>1</v>
@@ -4405,16 +4545,19 @@
         <v>1</v>
       </c>
       <c r="O33" s="33"/>
-      <c r="P33" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q33" s="15"/>
-    </row>
-    <row r="34" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="15"/>
+    </row>
+    <row r="34" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="23" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C34" s="14">
         <v>1</v>
@@ -4429,7 +4572,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -4445,16 +4588,19 @@
       <c r="O34" s="85">
         <v>1</v>
       </c>
-      <c r="P34" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="3"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P34" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R34" s="15"/>
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C35" s="14">
         <v>3</v>
@@ -4475,7 +4621,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
@@ -4495,13 +4641,16 @@
       <c r="O35" s="34">
         <v>1</v>
       </c>
-      <c r="P35" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q35" s="15"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P35" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R35" s="15"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
         <v>134</v>
       </c>
@@ -4533,14 +4682,17 @@
       <c r="O36" s="34">
         <v>0</v>
       </c>
-      <c r="P36" s="77">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="84"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P36" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="15"/>
+      <c r="S36" s="84"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
         <v>97</v>
       </c>
@@ -4577,14 +4729,17 @@
       <c r="O37" s="34">
         <v>1</v>
       </c>
-      <c r="P37" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="84"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P37" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R37" s="15"/>
+      <c r="S37" s="84"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
         <v>98</v>
       </c>
@@ -4598,7 +4753,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L38" s="20">
         <v>1</v>
@@ -4609,15 +4764,18 @@
       <c r="O38" s="34">
         <v>1</v>
       </c>
-      <c r="P38" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="84"/>
-      <c r="U38" s="6"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P38" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R38" s="15"/>
+      <c r="S38" s="84"/>
+      <c r="V38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
         <v>95</v>
       </c>
@@ -4631,7 +4789,7 @@
         <v>20</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L39" s="20">
         <v>1</v>
@@ -4642,13 +4800,16 @@
       <c r="O39" s="34">
         <v>1</v>
       </c>
-      <c r="P39" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q39" s="15"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P39" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R39" s="15"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
         <v>135</v>
       </c>
@@ -4689,15 +4850,18 @@
       <c r="O40" s="34">
         <v>1</v>
       </c>
-      <c r="P40" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q40" s="15"/>
+      <c r="P40" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R40" s="15"/>
-      <c r="S40" s="6"/>
-    </row>
-    <row r="41" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S40" s="15"/>
+      <c r="T40" s="6"/>
+    </row>
+    <row r="41" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>78</v>
       </c>
@@ -4711,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F41" s="13">
         <v>23</v>
@@ -4723,7 +4887,7 @@
         <v>22</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J41" s="12">
         <v>1</v>
@@ -4743,22 +4907,25 @@
       <c r="O41" s="35">
         <v>1</v>
       </c>
-      <c r="P41" s="78">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="3"/>
-      <c r="S41"/>
+      <c r="P41" s="88">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="15"/>
+      <c r="S41" s="3"/>
       <c r="T41"/>
-      <c r="V41"/>
+      <c r="U41"/>
       <c r="W41"/>
       <c r="X41"/>
       <c r="Y41"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z41"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B42" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C42" s="14">
         <v>5</v>
@@ -4797,19 +4964,22 @@
       <c r="O42" s="34">
         <v>1</v>
       </c>
-      <c r="P42" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q42" s="15"/>
-      <c r="V42" s="6"/>
+      <c r="P42" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R42" s="15"/>
       <c r="W42" s="6"/>
       <c r="X42" s="6"/>
       <c r="Y42" s="6"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z42" s="6"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C43" s="14">
         <v>4</v>
@@ -4818,18 +4988,21 @@
         <v>0</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="M43" s="34"/>
       <c r="O43" s="33"/>
-      <c r="P43" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="15"/>
-      <c r="U43" s="6"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P43" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="15"/>
+      <c r="V43" s="6"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="s">
         <v>137</v>
       </c>
@@ -4861,15 +5034,18 @@
       <c r="O44" s="34">
         <v>1</v>
       </c>
-      <c r="P44" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q44" s="15"/>
+      <c r="P44" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="Q44" s="77">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="R44" s="15"/>
-      <c r="S44" s="6"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="S44" s="15"/>
+      <c r="T44" s="6"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B45" s="23" t="s">
         <v>138</v>
       </c>
@@ -4880,7 +5056,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F45" s="14">
         <v>26</v>
@@ -4892,7 +5068,7 @@
         <v>25</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K45" s="2">
         <v>0.5</v>
@@ -4909,14 +5085,17 @@
       <c r="O45" s="34">
         <v>1</v>
       </c>
-      <c r="P45" s="77">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Q45" s="15"/>
-      <c r="T45" s="6"/>
-    </row>
-    <row r="46" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P45" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R45" s="15"/>
+      <c r="U45" s="6"/>
+    </row>
+    <row r="46" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>79</v>
       </c>
@@ -4930,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F46" s="13">
         <v>28</v>
@@ -4962,21 +5141,24 @@
       <c r="O46" s="35">
         <v>0.8</v>
       </c>
-      <c r="P46" s="78">
-        <f t="shared" si="1"/>
-        <v>3.8</v>
-      </c>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="3"/>
-      <c r="S46"/>
+      <c r="P46" s="88">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R46" s="15"/>
+      <c r="S46" s="3"/>
       <c r="T46"/>
       <c r="U46"/>
       <c r="V46"/>
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z46"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="s">
         <v>93</v>
       </c>
@@ -4987,7 +5169,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F47" s="14">
         <v>29</v>
@@ -5019,13 +5201,16 @@
       <c r="O47" s="34">
         <v>0.8</v>
       </c>
-      <c r="P47" s="77">
-        <f t="shared" si="1"/>
-        <v>3.7</v>
-      </c>
-      <c r="Q47" s="15"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P47" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R47" s="15"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="s">
         <v>139</v>
       </c>
@@ -5066,13 +5251,16 @@
       <c r="O48" s="34">
         <v>0.8</v>
       </c>
-      <c r="P48" s="77">
-        <f t="shared" si="1"/>
-        <v>3.2</v>
-      </c>
-      <c r="Q48" s="15"/>
-    </row>
-    <row r="49" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P48" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R48" s="15"/>
+    </row>
+    <row r="49" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>80</v>
       </c>
@@ -5108,19 +5296,22 @@
         <v>1</v>
       </c>
       <c r="O49" s="35"/>
-      <c r="P49" s="78">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q49" s="15"/>
+      <c r="P49" s="88">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="R49" s="15"/>
-      <c r="U49"/>
+      <c r="S49" s="15"/>
       <c r="V49"/>
       <c r="W49"/>
       <c r="X49"/>
       <c r="Y49"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z49"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B50" s="23" t="s">
         <v>141</v>
       </c>
@@ -5151,17 +5342,20 @@
         <v>1</v>
       </c>
       <c r="O50" s="34"/>
-      <c r="P50" s="77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q50" s="15"/>
-      <c r="V50" s="33"/>
-      <c r="W50" s="6"/>
+      <c r="P50" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R50" s="15"/>
+      <c r="W50" s="33"/>
       <c r="X50" s="6"/>
       <c r="Y50" s="6"/>
-    </row>
-    <row r="51" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Z50" s="6"/>
+    </row>
+    <row r="51" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>81</v>
       </c>
@@ -5197,21 +5391,24 @@
       <c r="O51" s="35">
         <v>0</v>
       </c>
-      <c r="P51" s="78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="3"/>
-      <c r="S51"/>
+      <c r="P51" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="Q51" s="78">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="R51" s="15"/>
+      <c r="S51" s="3"/>
       <c r="T51"/>
       <c r="U51"/>
-      <c r="V51" s="33"/>
-      <c r="W51"/>
+      <c r="V51"/>
+      <c r="W51" s="33"/>
       <c r="X51"/>
       <c r="Y51"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z51"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
         <v>143</v>
       </c>
@@ -5252,14 +5449,17 @@
       <c r="O52" s="85">
         <v>1</v>
       </c>
-      <c r="P52" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q52" s="15"/>
-      <c r="V52" s="33"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P52" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R52" s="15"/>
+      <c r="W52" s="33"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
         <v>144</v>
       </c>
@@ -5294,14 +5494,17 @@
       <c r="O53" s="85">
         <v>1</v>
       </c>
-      <c r="P53" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q53" s="15"/>
-      <c r="V53" s="33"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P53" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R53" s="15"/>
+      <c r="W53" s="33"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
         <v>145</v>
       </c>
@@ -5322,15 +5525,18 @@
       <c r="O54" s="85">
         <v>1</v>
       </c>
-      <c r="P54" s="77">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q54" s="15"/>
-      <c r="T54" s="6"/>
-      <c r="V54" s="33"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P54" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R54" s="15"/>
+      <c r="U54" s="6"/>
+      <c r="W54" s="33"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
         <v>146</v>
       </c>
@@ -5365,14 +5571,17 @@
       <c r="O55" s="85">
         <v>1</v>
       </c>
-      <c r="P55" s="77">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="Q55" s="15"/>
-      <c r="V55" s="33"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P55" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R55" s="15"/>
+      <c r="W55" s="33"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
         <v>147</v>
       </c>
@@ -5408,15 +5617,18 @@
         <v>1</v>
       </c>
       <c r="O56" s="33"/>
-      <c r="P56" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q56" s="15"/>
-      <c r="U56" s="6"/>
-      <c r="V56" s="33"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P56" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R56" s="15"/>
+      <c r="V56" s="6"/>
+      <c r="W56" s="33"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
         <v>148</v>
       </c>
@@ -5449,14 +5661,17 @@
         <v>1</v>
       </c>
       <c r="O57" s="33"/>
-      <c r="P57" s="77">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q57" s="15"/>
-      <c r="V57" s="33"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P57" s="87">
+        <v>0.6</v>
+      </c>
+      <c r="Q57" s="77">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="R57" s="15"/>
+      <c r="W57" s="33"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
         <v>149</v>
       </c>
@@ -5473,7 +5688,7 @@
         <v>35</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J58" s="2">
         <v>1</v>
@@ -5490,17 +5705,20 @@
       <c r="O58" s="85">
         <v>1</v>
       </c>
-      <c r="P58" s="77">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q58" s="15"/>
-      <c r="V58" s="33"/>
-      <c r="W58" s="6"/>
+      <c r="P58" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R58" s="15"/>
+      <c r="W58" s="33"/>
       <c r="X58" s="6"/>
       <c r="Y58" s="6"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z58" s="6"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
         <v>96</v>
       </c>
@@ -5514,7 +5732,7 @@
         <v>36</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L59" s="20">
         <v>0.5</v>
@@ -5523,14 +5741,17 @@
         <v>1</v>
       </c>
       <c r="O59" s="33"/>
-      <c r="P59" s="77">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="Q59" s="15"/>
-      <c r="V59" s="33"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P59" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R59" s="15"/>
+      <c r="W59" s="33"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
         <v>150</v>
       </c>
@@ -5555,15 +5776,18 @@
       <c r="O60" s="34">
         <v>0.5</v>
       </c>
-      <c r="P60" s="77">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="Q60" s="15"/>
-      <c r="U60" s="6"/>
-      <c r="V60" s="33"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P60" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R60" s="15"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="33"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
         <v>151</v>
       </c>
@@ -5582,14 +5806,17 @@
       </c>
       <c r="M61" s="34"/>
       <c r="O61" s="33"/>
-      <c r="P61" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q61" s="15"/>
-      <c r="V61" s="33"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P61" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R61" s="15"/>
+      <c r="W61" s="33"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
         <v>152</v>
       </c>
@@ -5605,13 +5832,16 @@
       <c r="I62" s="22"/>
       <c r="M62" s="34"/>
       <c r="O62" s="33"/>
-      <c r="P62" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q62" s="15"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P62" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R62" s="15"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
         <v>153</v>
       </c>
@@ -5625,7 +5855,7 @@
         <v>38</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="L63" s="20">
         <v>1</v>
@@ -5634,13 +5864,16 @@
         <v>1</v>
       </c>
       <c r="O63" s="34"/>
-      <c r="P63" s="77">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q63" s="15"/>
-    </row>
-    <row r="64" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P63" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="15"/>
+    </row>
+    <row r="64" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>82</v>
       </c>
@@ -5680,21 +5913,24 @@
         <v>1</v>
       </c>
       <c r="O64" s="35"/>
-      <c r="P64" s="78">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="3"/>
-      <c r="S64"/>
+      <c r="P64" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R64" s="15"/>
+      <c r="S64" s="3"/>
       <c r="T64"/>
       <c r="U64"/>
       <c r="V64"/>
       <c r="W64"/>
       <c r="X64"/>
       <c r="Y64"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z64"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B65" s="23" t="s">
         <v>155</v>
       </c>
@@ -5710,15 +5946,18 @@
       <c r="I65" s="22"/>
       <c r="M65" s="34"/>
       <c r="O65" s="33"/>
-      <c r="P65" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q65" s="15"/>
-      <c r="S65" s="33"/>
-      <c r="U65" s="6"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P65" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R65" s="15"/>
+      <c r="T65" s="33"/>
+      <c r="V65" s="6"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
         <v>156</v>
       </c>
@@ -5734,82 +5973,100 @@
       <c r="I66" s="22"/>
       <c r="M66" s="34"/>
       <c r="O66" s="33"/>
-      <c r="P66" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q66" s="15"/>
-      <c r="V66" s="6"/>
+      <c r="P66" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R66" s="15"/>
       <c r="W66" s="6"/>
       <c r="X66" s="6"/>
       <c r="Y66" s="6"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B67" s="23" t="s">
+      <c r="Z66" s="6"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A67" s="48"/>
+      <c r="B67" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="27">
         <v>10</v>
       </c>
-      <c r="D67" s="14">
-        <v>0</v>
-      </c>
-      <c r="E67" s="14">
+      <c r="D67" s="27">
+        <v>0</v>
+      </c>
+      <c r="E67" s="27">
         <v>34</v>
       </c>
-      <c r="I67" s="22"/>
-      <c r="K67" s="2">
-        <v>1</v>
-      </c>
-      <c r="M67" s="34"/>
-      <c r="O67" s="34"/>
-      <c r="P67" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q67" s="15"/>
-    </row>
-    <row r="68" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37">
+        <v>1</v>
+      </c>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="79">
+        <f t="shared" ref="Q67:Q76" si="4">SUM(P67)</f>
+        <v>0</v>
+      </c>
+      <c r="R67" s="15"/>
+    </row>
+    <row r="68" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="13">
-        <v>6</v>
-      </c>
-      <c r="D68" s="13">
-        <v>2</v>
-      </c>
-      <c r="E68" s="13">
-        <v>32</v>
-      </c>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="35"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="35"/>
-      <c r="P68" s="78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="3"/>
-      <c r="S68"/>
+      <c r="C68" s="14">
+        <v>4</v>
+      </c>
+      <c r="D68" s="14">
+        <v>0</v>
+      </c>
+      <c r="E68" s="14">
+        <v>48</v>
+      </c>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="34"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="33"/>
+      <c r="P68" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R68" s="15"/>
+      <c r="S68" s="3"/>
       <c r="T68"/>
       <c r="U68"/>
       <c r="V68"/>
       <c r="W68"/>
       <c r="X68"/>
       <c r="Y68"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z68"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B69" s="23" t="s">
         <v>159</v>
       </c>
@@ -5820,570 +6077,507 @@
         <v>0</v>
       </c>
       <c r="E69" s="14">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I69" s="22"/>
       <c r="M69" s="34"/>
-      <c r="O69" s="33"/>
-      <c r="P69" s="77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q69" s="15"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B70" s="23" t="s">
+      <c r="O69" s="34"/>
+      <c r="P69" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R69" s="15"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A70" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="C70" s="14">
-        <v>4</v>
-      </c>
-      <c r="D70" s="14">
-        <v>1</v>
-      </c>
-      <c r="E70" s="14">
-        <v>7</v>
-      </c>
-      <c r="I70" s="22"/>
-      <c r="M70" s="34"/>
-      <c r="O70" s="33"/>
-      <c r="P70" s="77">
-        <f t="shared" ref="P70:P80" si="5">SUM(L70:O70)</f>
-        <v>0</v>
-      </c>
-      <c r="Q70" s="15"/>
-      <c r="T70" s="33"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B71" s="23" t="s">
-        <v>161</v>
+      <c r="C70" s="13">
+        <v>2</v>
+      </c>
+      <c r="D70" s="13">
+        <v>0</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="12">
+        <v>1</v>
+      </c>
+      <c r="K70" s="12">
+        <v>1</v>
+      </c>
+      <c r="L70" s="12">
+        <v>1</v>
+      </c>
+      <c r="M70" s="35">
+        <v>1</v>
+      </c>
+      <c r="N70" s="12">
+        <v>1</v>
+      </c>
+      <c r="O70" s="35"/>
+      <c r="P70" s="88">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="78">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R70" s="15"/>
+      <c r="U70" s="33"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A71" s="30"/>
+      <c r="B71" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="C71" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D71" s="14">
-        <v>0</v>
-      </c>
-      <c r="E71" s="14">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="I71" s="22"/>
-      <c r="M71" s="34"/>
-      <c r="O71" s="33"/>
-      <c r="P71" s="77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q71" s="15"/>
-      <c r="V71" s="6"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="M71" s="36"/>
+      <c r="N71" s="20"/>
+      <c r="O71" s="36"/>
+      <c r="P71" s="89"/>
+      <c r="Q71" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R71" s="15"/>
       <c r="W71" s="6"/>
       <c r="X71" s="6"/>
       <c r="Y71" s="6"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z71" s="6"/>
+    </row>
+    <row r="72" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
       <c r="B72" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="14">
+        <v>4</v>
+      </c>
+      <c r="D72" s="14">
+        <v>3</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="2">
+        <v>1</v>
+      </c>
+      <c r="K72" s="2">
+        <v>1</v>
+      </c>
+      <c r="L72" s="20">
+        <v>1</v>
+      </c>
+      <c r="M72" s="34">
+        <v>1</v>
+      </c>
+      <c r="N72" s="2">
+        <v>1</v>
+      </c>
+      <c r="O72" s="33"/>
+      <c r="P72" s="87">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="77">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R72" s="15"/>
+      <c r="S72" s="3"/>
+      <c r="T72"/>
+      <c r="U72"/>
+      <c r="V72"/>
+      <c r="W72"/>
+      <c r="X72"/>
+      <c r="Y72"/>
+      <c r="Z72"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B73" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C72" s="14">
+      <c r="C73" s="14">
+        <v>1</v>
+      </c>
+      <c r="D73" s="14">
+        <v>0</v>
+      </c>
+      <c r="I73" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="K73" s="2">
+        <v>1</v>
+      </c>
+      <c r="L73" s="20">
+        <v>1</v>
+      </c>
+      <c r="M73" s="34">
+        <v>1</v>
+      </c>
+      <c r="N73" s="2">
+        <v>1</v>
+      </c>
+      <c r="O73" s="33"/>
+      <c r="P73" s="33"/>
+      <c r="Q73" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R73" s="15"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="6"/>
+      <c r="Y73" s="6"/>
+      <c r="Z73" s="6"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B74" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="14">
         <v>3</v>
       </c>
-      <c r="D72" s="14">
-        <v>0</v>
-      </c>
-      <c r="E72" s="14">
-        <v>49</v>
-      </c>
-      <c r="I72" s="22"/>
-      <c r="M72" s="34"/>
-      <c r="O72" s="34"/>
-      <c r="P72" s="77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q72" s="15"/>
-    </row>
-    <row r="73" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" s="13">
-        <v>2</v>
-      </c>
-      <c r="D73" s="13">
-        <v>0</v>
-      </c>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="12">
-        <v>1</v>
-      </c>
-      <c r="K73" s="12">
-        <v>1</v>
-      </c>
-      <c r="L73" s="12">
-        <v>1</v>
-      </c>
-      <c r="M73" s="35">
-        <v>1</v>
-      </c>
-      <c r="N73" s="12">
-        <v>1</v>
-      </c>
-      <c r="O73" s="35"/>
-      <c r="P73" s="78">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="Q73" s="15"/>
-      <c r="R73" s="3"/>
-      <c r="S73"/>
-      <c r="T73"/>
-      <c r="U73"/>
-      <c r="V73"/>
-      <c r="W73"/>
-      <c r="X73"/>
-      <c r="Y73"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A74" s="30"/>
-      <c r="B74" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" s="14">
-        <v>2</v>
-      </c>
       <c r="D74" s="14">
         <v>1</v>
       </c>
       <c r="I74" s="22"/>
-      <c r="J74" s="20"/>
-      <c r="K74" s="20"/>
-      <c r="M74" s="36"/>
-      <c r="N74" s="20"/>
-      <c r="O74" s="36"/>
-      <c r="P74" s="77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q74" s="15"/>
-      <c r="V74" s="6"/>
-      <c r="W74" s="6"/>
-      <c r="X74" s="6"/>
-      <c r="Y74" s="6"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M74" s="34"/>
+      <c r="O74" s="33"/>
+      <c r="P74" s="33"/>
+      <c r="Q74" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R74" s="15"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B75" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C75" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="22"/>
-      <c r="J75" s="2">
-        <v>1</v>
-      </c>
-      <c r="K75" s="2">
-        <v>1</v>
-      </c>
-      <c r="L75" s="20">
-        <v>1</v>
-      </c>
-      <c r="M75" s="34">
-        <v>1</v>
-      </c>
-      <c r="N75" s="2">
-        <v>1</v>
-      </c>
+      <c r="M75" s="34"/>
       <c r="O75" s="33"/>
-      <c r="P75" s="77">
+      <c r="P75" s="33"/>
+      <c r="Q75" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R75" s="15"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="6"/>
+      <c r="Y75" s="6"/>
+      <c r="Z75" s="6"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B76" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C76" s="27">
+        <v>4</v>
+      </c>
+      <c r="D76" s="27">
+        <v>0</v>
+      </c>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="28"/>
+      <c r="O76" s="37"/>
+      <c r="P76" s="37"/>
+      <c r="Q76" s="79">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R76" s="15"/>
+    </row>
+    <row r="77" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="11"/>
+      <c r="R77" s="15"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I78" s="64" t="s">
+        <v>175</v>
+      </c>
+      <c r="J78" s="65">
+        <f t="array" ref="J78">SUM($C2:$C76*(J2:J76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>83</v>
+      </c>
+      <c r="K78" s="65">
+        <f t="array" ref="K78">SUM($C2:$C76*(K2:K76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>69</v>
+      </c>
+      <c r="L78" s="65">
+        <f t="array" ref="L78">SUM($C2:$C76*(L2:L76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>123</v>
+      </c>
+      <c r="M78" s="65">
+        <f t="array" ref="M78">SUM($C2:$C76*(M2:M76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>129</v>
+      </c>
+      <c r="N78" s="65">
+        <f t="array" ref="N78">SUM($C2:$C76*(N2:N76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>111</v>
+      </c>
+      <c r="O78" s="66">
+        <f t="array" ref="O78">SUM($C2:$C76*(O2:O76&gt;=0.9)*($Q2:$Q76&gt;=$S$12))</f>
+        <v>93</v>
+      </c>
+      <c r="P78" s="68"/>
+      <c r="R78" s="15"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I79" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="J79" s="68">
+        <f t="array" ref="J79">SUM($C2:$C76*J2:J76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>84.5</v>
+      </c>
+      <c r="K79" s="68">
+        <f t="array" ref="K79">SUM($C2:$C76*K2:K76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>88.9</v>
+      </c>
+      <c r="L79" s="68">
+        <f t="array" ref="L79">SUM($C2:$C76*L2:L76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>126.89999999999999</v>
+      </c>
+      <c r="M79" s="68">
+        <f t="array" ref="M79">SUM($C2:$C76*M2:M76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>130</v>
+      </c>
+      <c r="N79" s="68">
+        <f t="array" ref="N79">SUM($C2:$C76*N2:N76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>111</v>
+      </c>
+      <c r="O79" s="69">
+        <f t="array" ref="O79">SUM($C2:$C76*O2:O76*($Q2:$Q76&gt;=$S$12))</f>
+        <v>103.39999999999999</v>
+      </c>
+      <c r="P79" s="68"/>
+      <c r="R79" s="15"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I80" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="J80" s="68">
+        <f t="array" ref="J80">SUM($C$2:$C$76*(J$2:J$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>86</v>
+      </c>
+      <c r="K80" s="68">
+        <f t="array" ref="K80">SUM($C$2:$C$76*(K$2:K$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>102</v>
+      </c>
+      <c r="L80" s="68">
+        <f t="array" ref="L80">SUM($C$2:$C$76*(L$2:L$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>136</v>
+      </c>
+      <c r="M80" s="68">
+        <f t="array" ref="M80">SUM($C$2:$C$76*(M$2:M$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>131</v>
+      </c>
+      <c r="N80" s="68">
+        <f t="array" ref="N80">SUM($C$2:$C$76*(N$2:N$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>111</v>
+      </c>
+      <c r="O80" s="69">
+        <f t="array" ref="O80">SUM($C$2:$C$76*(O$2:O$76&gt;=0.1)*($Q$2:$Q$76&gt;=$S$12))</f>
+        <v>106</v>
+      </c>
+      <c r="P80" s="68"/>
+      <c r="R80" s="15"/>
+      <c r="V80" s="33"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I81" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="J81" s="68">
+        <f t="shared" ref="J81:O81" si="5">LOOKUP($S$12,$S23:$S31,$T23:$T31)</f>
+        <v>154</v>
+      </c>
+      <c r="K81" s="68">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="Q75" s="15"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B76" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C76" s="14">
-        <v>4</v>
-      </c>
-      <c r="D76" s="14">
-        <v>3</v>
-      </c>
-      <c r="I76" s="22"/>
-      <c r="J76" s="2">
-        <v>1</v>
-      </c>
-      <c r="K76" s="2">
-        <v>1</v>
-      </c>
-      <c r="L76" s="20">
-        <v>1</v>
-      </c>
-      <c r="M76" s="34">
-        <v>1</v>
-      </c>
-      <c r="N76" s="2">
-        <v>1</v>
-      </c>
-      <c r="O76" s="33"/>
-      <c r="P76" s="77">
+        <v>154</v>
+      </c>
+      <c r="L81" s="68">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="Q76" s="15"/>
-      <c r="V76" s="6"/>
-      <c r="W76" s="6"/>
-      <c r="X76" s="6"/>
-      <c r="Y76" s="6"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B77" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C77" s="14">
-        <v>1</v>
-      </c>
-      <c r="D77" s="14">
-        <v>0</v>
-      </c>
-      <c r="I77" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="K77" s="2">
-        <v>1</v>
-      </c>
-      <c r="L77" s="20">
-        <v>1</v>
-      </c>
-      <c r="M77" s="34">
-        <v>1</v>
-      </c>
-      <c r="N77" s="2">
-        <v>1</v>
-      </c>
-      <c r="O77" s="33"/>
-      <c r="P77" s="77">
+        <v>154</v>
+      </c>
+      <c r="M81" s="68">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="Q77" s="15"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B78" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="14">
-        <v>3</v>
-      </c>
-      <c r="D78" s="14">
-        <v>1</v>
-      </c>
-      <c r="I78" s="22"/>
-      <c r="M78" s="34"/>
-      <c r="O78" s="33"/>
-      <c r="P78" s="77">
+        <v>154</v>
+      </c>
+      <c r="N81" s="68">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q78" s="15"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B79" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="C79" s="14">
-        <v>1</v>
-      </c>
-      <c r="D79" s="14">
-        <v>0</v>
-      </c>
-      <c r="I79" s="22"/>
-      <c r="M79" s="34"/>
-      <c r="O79" s="33"/>
-      <c r="P79" s="77">
+        <v>154</v>
+      </c>
+      <c r="O81" s="69">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q79" s="15"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B80" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C80" s="27">
-        <v>4</v>
-      </c>
-      <c r="D80" s="27">
-        <v>0</v>
-      </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="29"/>
-      <c r="J80" s="28"/>
-      <c r="K80" s="28"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="37"/>
-      <c r="N80" s="28"/>
-      <c r="O80" s="37"/>
-      <c r="P80" s="79">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q80" s="15"/>
-    </row>
-    <row r="81" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="11"/>
-      <c r="Q81" s="15"/>
-      <c r="U81" s="33"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I82" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="P81" s="68"/>
+      <c r="R81" s="15"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I82" s="67" t="s">
         <v>179</v>
       </c>
-      <c r="J82" s="65">
-        <f t="array" ref="J82">SUM($C2:$C80*(J2:J80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>85</v>
-      </c>
-      <c r="K82" s="65">
-        <f t="array" ref="K82">SUM($C2:$C80*(K2:K80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>71</v>
-      </c>
-      <c r="L82" s="65">
-        <f t="array" ref="L82">SUM($C2:$C80*(L2:L80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>144</v>
-      </c>
-      <c r="M82" s="65">
-        <f t="array" ref="M82">SUM($C2:$C80*(M2:M80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>156</v>
-      </c>
-      <c r="N82" s="65">
-        <f t="array" ref="N82">SUM($C2:$C80*(N2:N80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>118</v>
-      </c>
-      <c r="O82" s="66">
-        <f t="array" ref="O82">SUM($C2:$C80*(O2:O80&gt;=0.9)*($P2:$P80&gt;=$R$12))</f>
-        <v>104</v>
-      </c>
-      <c r="Q82" s="15"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I83" s="67" t="s">
-        <v>181</v>
-      </c>
-      <c r="J83" s="68">
-        <f t="array" ref="J83">SUM($C2:$C80*J2:J80*($P2:$P80&gt;=$R$12))</f>
-        <v>86.5</v>
-      </c>
-      <c r="K83" s="68">
-        <f t="array" ref="K83">SUM($C2:$C80*K2:K80*($P2:$P80&gt;=$R$12))</f>
-        <v>90.9</v>
-      </c>
-      <c r="L83" s="68">
-        <f t="array" ref="L83">SUM($C2:$C80*L2:L80*($P2:$P80&gt;=$R$12))</f>
-        <v>153.30000000000001</v>
-      </c>
-      <c r="M83" s="68">
-        <f t="array" ref="M83">SUM($C2:$C80*M2:M80*($P2:$P80&gt;=$R$12))</f>
-        <v>157</v>
-      </c>
-      <c r="N83" s="68">
-        <f t="array" ref="N83">SUM($C2:$C80*N2:N80*($P2:$P80&gt;=$R$12))</f>
-        <v>118</v>
-      </c>
-      <c r="O83" s="69">
-        <f t="array" ref="O83">SUM($C2:$C80*O2:O80*($P2:$P80&gt;=$R$12))</f>
-        <v>116.89999999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I84" s="67" t="s">
-        <v>180</v>
-      </c>
-      <c r="J84" s="68">
-        <f t="array" ref="J84">SUM($C$2:$C$80*(J$2:J$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>88</v>
-      </c>
-      <c r="K84" s="68">
-        <f t="array" ref="K84">SUM($C$2:$C$80*(K$2:K$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>104</v>
-      </c>
-      <c r="L84" s="68">
-        <f t="array" ref="L84">SUM($C$2:$C$80*(L$2:L$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>166</v>
-      </c>
-      <c r="M84" s="68">
-        <f t="array" ref="M84">SUM($C$2:$C$80*(M$2:M$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>158</v>
-      </c>
-      <c r="N84" s="68">
-        <f t="array" ref="N84">SUM($C$2:$C$80*(N$2:N$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>118</v>
-      </c>
-      <c r="O84" s="69">
-        <f t="array" ref="O84">SUM($C$2:$C$80*(O$2:O$80&gt;=0.1)*($P$2:$P$80&gt;=$R$12))</f>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I85" s="67" t="s">
-        <v>182</v>
-      </c>
-      <c r="J85" s="68">
-        <f t="shared" ref="J85:O85" si="6">LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>173</v>
-      </c>
-      <c r="K85" s="68">
+      <c r="J82" s="70">
+        <f t="shared" ref="J82:O82" si="6">J79/J81</f>
+        <v>0.54870129870129869</v>
+      </c>
+      <c r="K82" s="70">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="L85" s="68">
+        <v>0.57727272727272727</v>
+      </c>
+      <c r="L82" s="70">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="M85" s="68">
+        <v>0.824025974025974</v>
+      </c>
+      <c r="M82" s="70">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="N85" s="68">
+        <v>0.8441558441558441</v>
+      </c>
+      <c r="N82" s="70">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="O85" s="69">
+        <v>0.72077922077922074</v>
+      </c>
+      <c r="O82" s="71">
         <f t="shared" si="6"/>
-        <v>173</v>
-      </c>
-    </row>
-    <row r="86" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="10"/>
-      <c r="B86" s="23"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="67" t="s">
-        <v>183</v>
-      </c>
-      <c r="J86" s="70">
-        <f t="shared" ref="J86:O86" si="7">J83/J85</f>
-        <v>0.5</v>
-      </c>
-      <c r="K86" s="70">
-        <f t="shared" si="7"/>
-        <v>0.52543352601156068</v>
-      </c>
-      <c r="L86" s="70">
-        <f t="shared" si="7"/>
-        <v>0.88612716763005783</v>
-      </c>
-      <c r="M86" s="70">
-        <f t="shared" si="7"/>
-        <v>0.90751445086705207</v>
-      </c>
-      <c r="N86" s="70">
-        <f t="shared" si="7"/>
-        <v>0.68208092485549132</v>
-      </c>
-      <c r="O86" s="71">
-        <f t="shared" si="7"/>
-        <v>0.67572254335260107</v>
-      </c>
-      <c r="P86" s="3"/>
-      <c r="Q86" s="3"/>
-      <c r="R86" s="3"/>
-      <c r="S86"/>
-      <c r="T86"/>
-      <c r="U86"/>
-      <c r="V86"/>
-      <c r="W86"/>
-      <c r="X86"/>
-      <c r="Y86"/>
-    </row>
-    <row r="87" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="33"/>
-      <c r="I87" s="72" t="s">
+        <v>0.67142857142857137</v>
+      </c>
+      <c r="P82" s="70"/>
+    </row>
+    <row r="83" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="33"/>
+      <c r="I83" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="J87" s="73">
-        <f t="array" ref="J87">SUM($C2:$C80*J2:J80*($P2:$P80&lt;$R$12))</f>
+      <c r="J83" s="73">
+        <f t="array" ref="J83">SUM($C2:$C76*J2:J76*($Q2:$Q76&lt;$S$12))</f>
         <v>30</v>
       </c>
-      <c r="K87" s="73">
-        <f t="array" ref="K87">SUM($C2:$C80*K2:K80*($P2:$P80&lt;$R$12))</f>
+      <c r="K83" s="73">
+        <f t="array" ref="K83">SUM($C2:$C76*K2:K76*($Q2:$Q76&lt;$S$12))</f>
         <v>38.5</v>
       </c>
-      <c r="L87" s="73">
-        <f t="array" ref="L87">SUM($C2:$C80*L2:L80*($P2:$P80&lt;$R$12))</f>
-        <v>2.6</v>
-      </c>
-      <c r="M87" s="73">
-        <f t="array" ref="M87">SUM($C2:$C80*M2:M80*($P2:$P80&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="N87" s="73">
-        <f t="array" ref="N87">SUM($C2:$C80*N2:N80*($P2:$P80&lt;$R$12))</f>
-        <v>23.5</v>
-      </c>
-      <c r="O87" s="74">
-        <f t="array" ref="O87">SUM($C2:$C80*O2:O80*($P2:$P80&lt;$R$12))</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C88" s="33"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C89" s="33"/>
-      <c r="V89" s="6"/>
-      <c r="W89" s="6"/>
-      <c r="X89" s="6"/>
-      <c r="Y89" s="6"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C90" s="33"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V93" s="6"/>
-      <c r="W93" s="6"/>
-      <c r="X93" s="6"/>
-      <c r="Y93" s="6"/>
-    </row>
-    <row r="98" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V98" s="6"/>
-      <c r="W98" s="6"/>
-      <c r="X98" s="6"/>
-      <c r="Y98" s="6"/>
-    </row>
-    <row r="111" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V111" s="33"/>
-      <c r="W111" s="33"/>
-      <c r="X111" s="33"/>
-      <c r="Y111" s="33"/>
+      <c r="L83" s="73">
+        <f t="array" ref="L83">SUM($C2:$C76*L2:L76*($Q2:$Q76&lt;$S$12))</f>
+        <v>27</v>
+      </c>
+      <c r="M83" s="73">
+        <f t="array" ref="M83">SUM($C2:$C76*M2:M76*($Q2:$Q76&lt;$S$12))</f>
+        <v>25</v>
+      </c>
+      <c r="N83" s="73">
+        <f t="array" ref="N83">SUM($C2:$C76*N2:N76*($Q2:$Q76&lt;$S$12))</f>
+        <v>28.5</v>
+      </c>
+      <c r="O83" s="74">
+        <f t="array" ref="O83">SUM($C2:$C76*O2:O76*($Q2:$Q76&lt;$S$12))</f>
+        <v>20.5</v>
+      </c>
+      <c r="P83" s="68"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C84" s="33"/>
+    </row>
+    <row r="85" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="10"/>
+      <c r="B85" s="23"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="20"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="20"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="34"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85"/>
+      <c r="U85"/>
+      <c r="V85"/>
+      <c r="W85"/>
+      <c r="X85"/>
+      <c r="Y85"/>
+      <c r="Z85"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C86" s="33"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="W88" s="6"/>
+      <c r="X88" s="6"/>
+      <c r="Y88" s="6"/>
+      <c r="Z88" s="6"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="W92" s="6"/>
+      <c r="X92" s="6"/>
+      <c r="Y92" s="6"/>
+      <c r="Z92" s="6"/>
+    </row>
+    <row r="97" spans="23:26" x14ac:dyDescent="0.3">
+      <c r="W97" s="6"/>
+      <c r="X97" s="6"/>
+      <c r="Y97" s="6"/>
+      <c r="Z97" s="6"/>
+    </row>
+    <row r="110" spans="23:26" x14ac:dyDescent="0.3">
+      <c r="W110" s="33"/>
+      <c r="X110" s="33"/>
+      <c r="Y110" s="33"/>
+      <c r="Z110" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P80">
+  <conditionalFormatting sqref="B2:Q76">
     <cfRule type="expression" dxfId="2" priority="28" stopIfTrue="1">
-      <formula>$P2&gt;=(0.5+$R$12)</formula>
+      <formula>$Q2&gt;=(0.5+$S$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
-      <formula>$P2&gt;=$R$12</formula>
+      <formula>$Q2&gt;=$S$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="30">
-      <formula>$P2&gt;=($R$12-0.5)</formula>
+      <formula>$Q2&gt;=($S$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>